<commit_message>
Updated timeline and created a presentationg document to help structure presentations, added section for architecture presentation
</commit_message>
<xml_diff>
--- a/GANTT chart.xlsx
+++ b/GANTT chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\black\Documents\School Stuff\2nd Year\CS 2043\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Year2\Fall\CS2043\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50BA07E-A997-4FDC-A2E0-41373E696BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524AC93F-4617-44D7-8EE8-359F6DF50B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -2939,6 +2939,33 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2946,39 +2973,12 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3221,13 +3221,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>99060</xdr:colOff>
+          <xdr:colOff>95250</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>121920</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>106680</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
@@ -3812,25 +3812,25 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomLeft" activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" style="6" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="1.88671875" style="1" customWidth="1"/>
-    <col min="11" max="66" width="2.44140625" style="1" customWidth="1"/>
-    <col min="67" max="16384" width="9.109375" style="3"/>
+    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.85546875" style="1" customWidth="1"/>
+    <col min="11" max="66" width="2.42578125" style="1" customWidth="1"/>
+    <col min="67" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="123" t="s">
         <v>1</v>
       </c>
@@ -3840,31 +3840,31 @@
       <c r="E1" s="46"/>
       <c r="F1" s="46"/>
       <c r="I1" s="130"/>
-      <c r="K1" s="163" t="s">
+      <c r="K1" s="172" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
-      <c r="P1" s="163"/>
-      <c r="Q1" s="163"/>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
-    </row>
-    <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="172"/>
+      <c r="M1" s="172"/>
+      <c r="N1" s="172"/>
+      <c r="O1" s="172"/>
+      <c r="P1" s="172"/>
+      <c r="Q1" s="172"/>
+      <c r="R1" s="172"/>
+      <c r="S1" s="172"/>
+      <c r="T1" s="172"/>
+      <c r="U1" s="172"/>
+      <c r="V1" s="172"/>
+      <c r="W1" s="172"/>
+      <c r="X1" s="172"/>
+      <c r="Y1" s="172"/>
+      <c r="Z1" s="172"/>
+      <c r="AA1" s="172"/>
+      <c r="AB1" s="172"/>
+      <c r="AC1" s="172"/>
+      <c r="AD1" s="172"/>
+      <c r="AE1" s="172"/>
+    </row>
+    <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
         <v>139</v>
       </c>
@@ -3875,7 +3875,7 @@
       <c r="F2" s="158"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:66" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="51"/>
       <c r="B3" s="47"/>
       <c r="C3" s="4"/>
@@ -3902,16 +3902,16 @@
       <c r="Z3" s="29"/>
       <c r="AA3" s="29"/>
     </row>
-    <row r="4" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="108"/>
       <c r="B4" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="168">
+      <c r="C4" s="174">
         <v>44151</v>
       </c>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="109"/>
       <c r="G4" s="112" t="s">
         <v>76</v>
@@ -3921,95 +3921,95 @@
       </c>
       <c r="I4" s="110"/>
       <c r="J4" s="49"/>
-      <c r="K4" s="165" t="str">
+      <c r="K4" s="166" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="166"/>
-      <c r="M4" s="166"/>
-      <c r="N4" s="166"/>
-      <c r="O4" s="166"/>
-      <c r="P4" s="166"/>
-      <c r="Q4" s="167"/>
-      <c r="R4" s="165" t="str">
+      <c r="L4" s="167"/>
+      <c r="M4" s="167"/>
+      <c r="N4" s="167"/>
+      <c r="O4" s="167"/>
+      <c r="P4" s="167"/>
+      <c r="Q4" s="168"/>
+      <c r="R4" s="166" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="166"/>
-      <c r="T4" s="166"/>
-      <c r="U4" s="166"/>
-      <c r="V4" s="166"/>
-      <c r="W4" s="166"/>
-      <c r="X4" s="167"/>
-      <c r="Y4" s="165" t="str">
+      <c r="S4" s="167"/>
+      <c r="T4" s="167"/>
+      <c r="U4" s="167"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="168"/>
+      <c r="Y4" s="166" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="166"/>
-      <c r="AA4" s="166"/>
-      <c r="AB4" s="166"/>
-      <c r="AC4" s="166"/>
-      <c r="AD4" s="166"/>
-      <c r="AE4" s="167"/>
-      <c r="AF4" s="165" t="str">
+      <c r="Z4" s="167"/>
+      <c r="AA4" s="167"/>
+      <c r="AB4" s="167"/>
+      <c r="AC4" s="167"/>
+      <c r="AD4" s="167"/>
+      <c r="AE4" s="168"/>
+      <c r="AF4" s="166" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="166"/>
-      <c r="AH4" s="166"/>
-      <c r="AI4" s="166"/>
-      <c r="AJ4" s="166"/>
-      <c r="AK4" s="166"/>
-      <c r="AL4" s="167"/>
-      <c r="AM4" s="165" t="str">
+      <c r="AG4" s="167"/>
+      <c r="AH4" s="167"/>
+      <c r="AI4" s="167"/>
+      <c r="AJ4" s="167"/>
+      <c r="AK4" s="167"/>
+      <c r="AL4" s="168"/>
+      <c r="AM4" s="166" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="166"/>
-      <c r="AO4" s="166"/>
-      <c r="AP4" s="166"/>
-      <c r="AQ4" s="166"/>
-      <c r="AR4" s="166"/>
-      <c r="AS4" s="167"/>
-      <c r="AT4" s="165" t="str">
+      <c r="AN4" s="167"/>
+      <c r="AO4" s="167"/>
+      <c r="AP4" s="167"/>
+      <c r="AQ4" s="167"/>
+      <c r="AR4" s="167"/>
+      <c r="AS4" s="168"/>
+      <c r="AT4" s="166" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="166"/>
-      <c r="AV4" s="166"/>
-      <c r="AW4" s="166"/>
-      <c r="AX4" s="166"/>
-      <c r="AY4" s="166"/>
-      <c r="AZ4" s="167"/>
-      <c r="BA4" s="165" t="str">
+      <c r="AU4" s="167"/>
+      <c r="AV4" s="167"/>
+      <c r="AW4" s="167"/>
+      <c r="AX4" s="167"/>
+      <c r="AY4" s="167"/>
+      <c r="AZ4" s="168"/>
+      <c r="BA4" s="166" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="166"/>
-      <c r="BC4" s="166"/>
-      <c r="BD4" s="166"/>
-      <c r="BE4" s="166"/>
-      <c r="BF4" s="166"/>
-      <c r="BG4" s="167"/>
-      <c r="BH4" s="165" t="str">
+      <c r="BB4" s="167"/>
+      <c r="BC4" s="167"/>
+      <c r="BD4" s="167"/>
+      <c r="BE4" s="167"/>
+      <c r="BF4" s="167"/>
+      <c r="BG4" s="168"/>
+      <c r="BH4" s="166" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="166"/>
-      <c r="BJ4" s="166"/>
-      <c r="BK4" s="166"/>
-      <c r="BL4" s="166"/>
-      <c r="BM4" s="166"/>
-      <c r="BN4" s="167"/>
-    </row>
-    <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI4" s="167"/>
+      <c r="BJ4" s="167"/>
+      <c r="BK4" s="167"/>
+      <c r="BL4" s="167"/>
+      <c r="BM4" s="167"/>
+      <c r="BN4" s="168"/>
+    </row>
+    <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="108"/>
       <c r="B5" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="164"/>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
+      <c r="C5" s="173"/>
+      <c r="D5" s="173"/>
+      <c r="E5" s="173"/>
       <c r="F5" s="111"/>
       <c r="G5" s="111"/>
       <c r="H5" s="111"/>
@@ -4096,7 +4096,7 @@
       <c r="BM5" s="170"/>
       <c r="BN5" s="171"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
       <c r="B6" s="49"/>
       <c r="C6" s="49"/>
@@ -4332,7 +4332,7 @@
         <v>44206</v>
       </c>
     </row>
-    <row r="7" spans="1:66" s="122" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:66" s="122" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="114" t="s">
         <v>0</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="8" spans="1:66" s="54" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="83" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -4598,13 +4598,13 @@
       <c r="D8" s="86"/>
       <c r="E8" s="87"/>
       <c r="F8" s="113" t="str">
-        <f>IF(ISBLANK(E8)," - ",IF(G8=0,E8,E8+G8-1))</f>
+        <f t="shared" ref="F8:F24" si="4">IF(ISBLANK(E8)," - ",IF(G8=0,E8,E8+G8-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G8" s="88"/>
       <c r="H8" s="89"/>
       <c r="I8" s="90" t="str">
-        <f>IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I23" si="5">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="93"/>
@@ -4665,7 +4665,7 @@
       <c r="BM8" s="105"/>
       <c r="BN8" s="105"/>
     </row>
-    <row r="9" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -4681,7 +4681,7 @@
         <v>44146</v>
       </c>
       <c r="F9" s="100">
-        <f>IF(ISBLANK(E9)," - ",IF(G9=0,E9,E9+G9-1))</f>
+        <f t="shared" si="4"/>
         <v>44150</v>
       </c>
       <c r="G9" s="61">
@@ -4691,7 +4691,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="63">
-        <f>IF(OR(F9=0,E9=0)," - ",NETWORKDAYS(E9,F9))</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J9" s="94"/>
@@ -4752,7 +4752,7 @@
       <c r="BM9" s="106"/>
       <c r="BN9" s="106"/>
     </row>
-    <row r="10" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.2</v>
@@ -4765,7 +4765,7 @@
         <v>44150</v>
       </c>
       <c r="F10" s="100">
-        <f>IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
+        <f t="shared" si="4"/>
         <v>44152</v>
       </c>
       <c r="G10" s="61">
@@ -4775,7 +4775,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="63">
-        <f>IF(OR(F10=0,E10=0)," - ",NETWORKDAYS(E10,F10))</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="J10" s="94"/>
@@ -4836,7 +4836,7 @@
       <c r="BM10" s="106"/>
       <c r="BN10" s="106"/>
     </row>
-    <row r="11" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.3</v>
@@ -4849,7 +4849,7 @@
         <v>44152</v>
       </c>
       <c r="F11" s="100">
-        <f>IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
+        <f t="shared" si="4"/>
         <v>44152</v>
       </c>
       <c r="G11" s="61">
@@ -4859,7 +4859,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="63">
-        <f>IF(OR(F11=0,E11=0)," - ",NETWORKDAYS(E11,F11))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J11" s="94"/>
@@ -4920,7 +4920,7 @@
       <c r="BM11" s="106"/>
       <c r="BN11" s="106"/>
     </row>
-    <row r="12" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.1</v>
@@ -4933,7 +4933,7 @@
         <v>44152</v>
       </c>
       <c r="F12" s="100">
-        <f>IF(ISBLANK(E12)," - ",IF(G12=0,E12,E12+G12-1))</f>
+        <f t="shared" si="4"/>
         <v>44152</v>
       </c>
       <c r="G12" s="61">
@@ -4943,7 +4943,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="63">
-        <f>IF(OR(F12=0,E12=0)," - ",NETWORKDAYS(E12,F12))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J12" s="94"/>
@@ -5004,7 +5004,7 @@
       <c r="BM12" s="106"/>
       <c r="BN12" s="106"/>
     </row>
-    <row r="13" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.2</v>
@@ -5017,7 +5017,7 @@
         <v>44153</v>
       </c>
       <c r="F13" s="100">
-        <f>IF(ISBLANK(E13)," - ",IF(G13=0,E13,E13+G13-1))</f>
+        <f t="shared" si="4"/>
         <v>44153</v>
       </c>
       <c r="G13" s="61">
@@ -5027,7 +5027,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="63">
-        <f>IF(OR(F13=0,E13=0)," - ",NETWORKDAYS(E13,F13))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J13" s="94"/>
@@ -5088,7 +5088,7 @@
       <c r="BM13" s="106"/>
       <c r="BN13" s="106"/>
     </row>
-    <row r="14" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.3</v>
@@ -5101,7 +5101,7 @@
         <v>44153</v>
       </c>
       <c r="F14" s="100">
-        <f>IF(ISBLANK(E14)," - ",IF(G14=0,E14,E14+G14-1))</f>
+        <f t="shared" si="4"/>
         <v>44153</v>
       </c>
       <c r="G14" s="61">
@@ -5111,7 +5111,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="63">
-        <f>IF(OR(F14=0,E14=0)," - ",NETWORKDAYS(E14,F14))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J14" s="94"/>
@@ -5172,7 +5172,7 @@
       <c r="BM14" s="106"/>
       <c r="BN14" s="106"/>
     </row>
-    <row r="15" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.4</v>
@@ -5185,17 +5185,17 @@
         <v>44154</v>
       </c>
       <c r="F15" s="100">
-        <f>IF(ISBLANK(E15)," - ",IF(G15=0,E15,E15+G15-1))</f>
+        <f t="shared" si="4"/>
         <v>44156</v>
       </c>
       <c r="G15" s="61">
         <v>3</v>
       </c>
       <c r="H15" s="62">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I15" s="63">
-        <f>IF(OR(F15=0,E15=0)," - ",NETWORKDAYS(E15,F15))</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="J15" s="94"/>
@@ -5256,7 +5256,7 @@
       <c r="BM15" s="106"/>
       <c r="BN15" s="106"/>
     </row>
-    <row r="16" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.5</v>
@@ -5269,17 +5269,17 @@
         <v>44154</v>
       </c>
       <c r="F16" s="100">
-        <f>IF(ISBLANK(E16)," - ",IF(G16=0,E16,E16+G16-1))</f>
+        <f t="shared" si="4"/>
         <v>44157</v>
       </c>
       <c r="G16" s="61">
         <v>4</v>
       </c>
       <c r="H16" s="62">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I16" s="63">
-        <f>IF(OR(F16=0,E16=0)," - ",NETWORKDAYS(E16,F16))</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="J16" s="94"/>
@@ -5340,7 +5340,7 @@
       <c r="BM16" s="106"/>
       <c r="BN16" s="106"/>
     </row>
-    <row r="17" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.6</v>
@@ -5353,17 +5353,17 @@
         <v>44156</v>
       </c>
       <c r="F17" s="100">
-        <f>IF(ISBLANK(E17)," - ",IF(G17=0,E17,E17+G17-1))</f>
+        <f t="shared" si="4"/>
         <v>44157</v>
       </c>
       <c r="G17" s="61">
         <v>2</v>
       </c>
       <c r="H17" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="63">
-        <f>IF(OR(F17=0,E17=0)," - ",NETWORKDAYS(E17,F17))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J17" s="94"/>
@@ -5424,7 +5424,7 @@
       <c r="BM17" s="106"/>
       <c r="BN17" s="106"/>
     </row>
-    <row r="18" spans="1:66" s="54" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="52" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -5435,13 +5435,13 @@
       <c r="D18" s="55"/>
       <c r="E18" s="101"/>
       <c r="F18" s="101" t="str">
-        <f>IF(ISBLANK(E18)," - ",IF(G18=0,E18,E18+G18-1))</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G18" s="56"/>
       <c r="H18" s="57"/>
       <c r="I18" s="58" t="str">
-        <f>IF(OR(F18=0,E18=0)," - ",NETWORKDAYS(E18,F18))</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J18" s="95"/>
@@ -5502,9 +5502,9 @@
       <c r="BM18" s="107"/>
       <c r="BN18" s="107"/>
     </row>
-    <row r="19" spans="1:66" s="60" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A19:A24" si="6">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
       <c r="B19" s="162" t="s">
@@ -5515,17 +5515,17 @@
         <v>44153</v>
       </c>
       <c r="F19" s="100">
-        <f>IF(ISBLANK(E19)," - ",IF(G19=0,E19,E19+G19-1))</f>
+        <f t="shared" si="4"/>
         <v>44153</v>
       </c>
       <c r="G19" s="61">
         <v>1</v>
       </c>
       <c r="H19" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="63">
-        <f>IF(OR(F19=0,E19=0)," - ",NETWORKDAYS(E19,F19))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J19" s="94"/>
@@ -5586,9 +5586,9 @@
       <c r="BM19" s="106"/>
       <c r="BN19" s="106"/>
     </row>
-    <row r="20" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="6"/>
         <v>2.2</v>
       </c>
       <c r="B20" s="124" t="s">
@@ -5599,17 +5599,17 @@
         <v>44154</v>
       </c>
       <c r="F20" s="100">
-        <f>IF(ISBLANK(E20)," - ",IF(G20=0,E20,E20+G20-1))</f>
+        <f t="shared" si="4"/>
         <v>44154</v>
       </c>
       <c r="G20" s="61">
         <v>1</v>
       </c>
       <c r="H20" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="63">
-        <f>IF(OR(F20=0,E20=0)," - ",NETWORKDAYS(E20,F20))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J20" s="94"/>
@@ -5670,9 +5670,9 @@
       <c r="BM20" s="106"/>
       <c r="BN20" s="106"/>
     </row>
-    <row r="21" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="6"/>
         <v>2.3</v>
       </c>
       <c r="B21" s="124" t="s">
@@ -5683,17 +5683,17 @@
         <v>44154</v>
       </c>
       <c r="F21" s="100">
-        <f>IF(ISBLANK(E21)," - ",IF(G21=0,E21,E21+G21-1))</f>
+        <f t="shared" si="4"/>
         <v>44154</v>
       </c>
       <c r="G21" s="61">
         <v>1</v>
       </c>
       <c r="H21" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="63">
-        <f>IF(OR(F21=0,E21=0)," - ",NETWORKDAYS(E21,F21))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J21" s="94"/>
@@ -5754,9 +5754,9 @@
       <c r="BM21" s="106"/>
       <c r="BN21" s="106"/>
     </row>
-    <row r="22" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="6"/>
         <v>2.4</v>
       </c>
       <c r="B22" s="124" t="s">
@@ -5767,17 +5767,17 @@
         <v>44154</v>
       </c>
       <c r="F22" s="100">
-        <f>IF(ISBLANK(E22)," - ",IF(G22=0,E22,E22+G22-1))</f>
+        <f t="shared" si="4"/>
         <v>44155</v>
       </c>
       <c r="G22" s="61">
         <v>2</v>
       </c>
       <c r="H22" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="63">
-        <f>IF(OR(F22=0,E22=0)," - ",NETWORKDAYS(E22,F22))</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="J22" s="94"/>
@@ -5838,9 +5838,9 @@
       <c r="BM22" s="106"/>
       <c r="BN22" s="106"/>
     </row>
-    <row r="23" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="B23" s="124" t="s">
@@ -5851,17 +5851,17 @@
         <v>44155</v>
       </c>
       <c r="F23" s="100">
-        <f>IF(ISBLANK(E23)," - ",IF(G23=0,E23,E23+G23-1))</f>
+        <f t="shared" si="4"/>
         <v>44156</v>
       </c>
       <c r="G23" s="61">
         <v>2</v>
       </c>
       <c r="H23" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="63">
-        <f>IF(OR(F23=0,E23=0)," - ",NETWORKDAYS(E23,F23))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J23" s="94"/>
@@ -5922,32 +5922,32 @@
       <c r="BM23" s="106"/>
       <c r="BN23" s="106"/>
     </row>
-    <row r="24" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="6"/>
         <v>2.6</v>
       </c>
       <c r="B24" s="124" t="s">
         <v>158</v>
       </c>
-      <c r="D24" s="173"/>
+      <c r="D24" s="163"/>
       <c r="E24" s="99">
         <v>44155</v>
       </c>
       <c r="F24" s="100">
-        <f>IF(ISBLANK(E24)," - ",IF(G24=0,E24,E24+G24-1))</f>
+        <f t="shared" si="4"/>
         <v>44156</v>
       </c>
       <c r="G24" s="61">
         <v>2</v>
       </c>
       <c r="H24" s="62">
-        <v>0</v>
-      </c>
-      <c r="I24" s="174">
         <v>1</v>
       </c>
-      <c r="J24" s="175"/>
+      <c r="I24" s="164">
+        <v>1</v>
+      </c>
+      <c r="J24" s="165"/>
       <c r="K24" s="106"/>
       <c r="L24" s="106"/>
       <c r="M24" s="106"/>
@@ -6005,7 +6005,7 @@
       <c r="BM24" s="106"/>
       <c r="BN24" s="106"/>
     </row>
-    <row r="25" spans="1:66" s="54" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="52" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
@@ -6016,13 +6016,13 @@
       <c r="D25" s="55"/>
       <c r="E25" s="101"/>
       <c r="F25" s="101" t="str">
-        <f t="shared" ref="F11:F35" si="4">IF(ISBLANK(E25)," - ",IF(G25=0,E25,E25+G25-1))</f>
+        <f t="shared" ref="F25:F35" si="7">IF(ISBLANK(E25)," - ",IF(G25=0,E25,E25+G25-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G25" s="56"/>
       <c r="H25" s="57"/>
       <c r="I25" s="58" t="str">
-        <f t="shared" ref="I8:I38" si="5">IF(OR(F25=0,E25=0)," - ",NETWORKDAYS(E25,F25))</f>
+        <f t="shared" ref="I25:I38" si="8">IF(OR(F25=0,E25=0)," - ",NETWORKDAYS(E25,F25))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J25" s="95"/>
@@ -6083,7 +6083,7 @@
       <c r="BM25" s="107"/>
       <c r="BN25" s="107"/>
     </row>
-    <row r="26" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
@@ -6096,7 +6096,7 @@
         <v>44157</v>
       </c>
       <c r="F26" s="100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>44159</v>
       </c>
       <c r="G26" s="61">
@@ -6106,7 +6106,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="J26" s="94"/>
@@ -6167,7 +6167,7 @@
       <c r="BM26" s="106"/>
       <c r="BN26" s="106"/>
     </row>
-    <row r="27" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.2</v>
@@ -6180,7 +6180,7 @@
         <v>44158</v>
       </c>
       <c r="F27" s="100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>44159</v>
       </c>
       <c r="G27" s="61">
@@ -6190,7 +6190,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="J27" s="94"/>
@@ -6251,7 +6251,7 @@
       <c r="BM27" s="106"/>
       <c r="BN27" s="106"/>
     </row>
-    <row r="28" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.3</v>
@@ -6264,7 +6264,7 @@
         <v>44159</v>
       </c>
       <c r="F28" s="100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>44161</v>
       </c>
       <c r="G28" s="61">
@@ -6274,7 +6274,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J28" s="94"/>
@@ -6335,7 +6335,7 @@
       <c r="BM28" s="106"/>
       <c r="BN28" s="106"/>
     </row>
-    <row r="29" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.4</v>
@@ -6348,7 +6348,7 @@
         <v>44160</v>
       </c>
       <c r="F29" s="100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>44162</v>
       </c>
       <c r="G29" s="61">
@@ -6358,7 +6358,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J29" s="94"/>
@@ -6419,7 +6419,7 @@
       <c r="BM29" s="106"/>
       <c r="BN29" s="106"/>
     </row>
-    <row r="30" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.5</v>
@@ -6432,7 +6432,7 @@
         <v>44161</v>
       </c>
       <c r="F30" s="100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>44164</v>
       </c>
       <c r="G30" s="61">
@@ -6442,7 +6442,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="J30" s="94"/>
@@ -6503,7 +6503,7 @@
       <c r="BM30" s="106"/>
       <c r="BN30" s="106"/>
     </row>
-    <row r="31" spans="1:66" s="54" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="52" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
@@ -6514,13 +6514,13 @@
       <c r="D31" s="55"/>
       <c r="E31" s="101"/>
       <c r="F31" s="101" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G31" s="56"/>
       <c r="H31" s="57"/>
       <c r="I31" s="58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J31" s="95"/>
@@ -6581,7 +6581,7 @@
       <c r="BM31" s="107"/>
       <c r="BN31" s="107"/>
     </row>
-    <row r="32" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
@@ -6604,7 +6604,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="J32" s="94"/>
@@ -6665,7 +6665,7 @@
       <c r="BM32" s="106"/>
       <c r="BN32" s="106"/>
     </row>
-    <row r="33" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.2</v>
@@ -6678,7 +6678,7 @@
         <v>44168</v>
       </c>
       <c r="F33" s="100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>44168</v>
       </c>
       <c r="G33" s="61">
@@ -6688,7 +6688,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="J33" s="94"/>
@@ -6749,7 +6749,7 @@
       <c r="BM33" s="106"/>
       <c r="BN33" s="106"/>
     </row>
-    <row r="34" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.3</v>
@@ -6762,7 +6762,7 @@
         <v>44169</v>
       </c>
       <c r="F34" s="100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>44169</v>
       </c>
       <c r="G34" s="61">
@@ -6772,7 +6772,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="J34" s="94"/>
@@ -6833,7 +6833,7 @@
       <c r="BM34" s="106"/>
       <c r="BN34" s="106"/>
     </row>
-    <row r="35" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.4</v>
@@ -6846,7 +6846,7 @@
         <v>44170</v>
       </c>
       <c r="F35" s="100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>44170</v>
       </c>
       <c r="G35" s="61">
@@ -6856,7 +6856,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J35" s="94"/>
@@ -6917,7 +6917,7 @@
       <c r="BM35" s="106"/>
       <c r="BN35" s="106"/>
     </row>
-    <row r="36" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.5</v>
@@ -6940,7 +6940,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J36" s="94"/>
@@ -7001,7 +7001,7 @@
       <c r="BM36" s="106"/>
       <c r="BN36" s="106"/>
     </row>
-    <row r="37" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="59"/>
       <c r="B37" s="64"/>
       <c r="C37" s="64"/>
@@ -7011,7 +7011,7 @@
       <c r="G37" s="66"/>
       <c r="H37" s="67"/>
       <c r="I37" s="68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J37" s="96"/>
@@ -7072,7 +7072,7 @@
       <c r="BM37" s="106"/>
       <c r="BN37" s="106"/>
     </row>
-    <row r="38" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="59"/>
       <c r="B38" s="64"/>
       <c r="C38" s="64"/>
@@ -7082,7 +7082,7 @@
       <c r="G38" s="66"/>
       <c r="H38" s="67"/>
       <c r="I38" s="68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J38" s="96"/>
@@ -7143,7 +7143,7 @@
       <c r="BM38" s="106"/>
       <c r="BN38" s="106"/>
     </row>
-    <row r="39" spans="1:66" s="74" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:66" s="74" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="70" t="s">
         <v>2</v>
       </c>
@@ -7213,7 +7213,7 @@
       <c r="BM39" s="106"/>
       <c r="BN39" s="106"/>
     </row>
-    <row r="40" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="75" t="s">
         <v>40</v>
       </c>
@@ -7283,7 +7283,7 @@
       <c r="BM40" s="106"/>
       <c r="BN40" s="106"/>
     </row>
-    <row r="41" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="128" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -7295,7 +7295,7 @@
       <c r="D41" s="78"/>
       <c r="E41" s="99"/>
       <c r="F41" s="100" t="str">
-        <f t="shared" ref="F41:F44" si="6">IF(ISBLANK(E41)," - ",IF(G41=0,E41,E41+G41-1))</f>
+        <f t="shared" ref="F41:F44" si="9">IF(ISBLANK(E41)," - ",IF(G41=0,E41,E41+G41-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G41" s="61"/>
@@ -7362,7 +7362,7 @@
       <c r="BM41" s="106"/>
       <c r="BN41" s="106"/>
     </row>
-    <row r="42" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -7374,13 +7374,13 @@
       <c r="D42" s="78"/>
       <c r="E42" s="99"/>
       <c r="F42" s="100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G42" s="61"/>
       <c r="H42" s="62"/>
       <c r="I42" s="79" t="str">
-        <f t="shared" ref="I42:I44" si="7">IF(OR(F42=0,E42=0)," - ",NETWORKDAYS(E42,F42))</f>
+        <f t="shared" ref="I42:I44" si="10">IF(OR(F42=0,E42=0)," - ",NETWORKDAYS(E42,F42))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J42" s="98"/>
@@ -7441,7 +7441,7 @@
       <c r="BM42" s="106"/>
       <c r="BN42" s="106"/>
     </row>
-    <row r="43" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -7453,13 +7453,13 @@
       <c r="D43" s="78"/>
       <c r="E43" s="99"/>
       <c r="F43" s="100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G43" s="61"/>
       <c r="H43" s="62"/>
       <c r="I43" s="79" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J43" s="98"/>
@@ -7520,7 +7520,7 @@
       <c r="BM43" s="106"/>
       <c r="BN43" s="106"/>
     </row>
-    <row r="44" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>1.1.1.1</v>
@@ -7532,13 +7532,13 @@
       <c r="D44" s="78"/>
       <c r="E44" s="99"/>
       <c r="F44" s="100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G44" s="61"/>
       <c r="H44" s="62"/>
       <c r="I44" s="79" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J44" s="98"/>
@@ -7599,7 +7599,7 @@
       <c r="BM44" s="106"/>
       <c r="BN44" s="106"/>
     </row>
-    <row r="45" spans="1:66" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:66" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="161" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToCreateAGanttChart","► Watch How to Create a Gantt Chart in Excel")</f>
         <v>► Watch How to Create a Gantt Chart in Excel</v>
@@ -7673,6 +7673,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7683,15 +7692,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H44">
@@ -7736,7 +7736,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A37:B38 B32 B33:B35 B27:B29 A40:B40 B39 E18 E25 E31 E38:H40 G18:H18 G25:H25 G31:H35 H22 G41 G42:G43 G44 H20 H21 H26:H29 F37:H37" unlockedFormula="1"/>
+    <ignoredError sqref="H9 A37:B38 B32 B33:B35 B27:B29 A40:B40 B39 E18 E25 E31 E38:H40 G18:H18 G25:H25 G31:H35 G41 G42:G43 G44 H26:H29 F37:H37" unlockedFormula="1"/>
     <ignoredError sqref="A31 A25 A18" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
@@ -7751,13 +7751,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>99060</xdr:colOff>
+                    <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>121920</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>27</xdr:col>
-                    <xdr:colOff>106680</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </to>
@@ -7804,175 +7804,175 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="55.109375" style="16" customWidth="1"/>
-    <col min="4" max="7" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="5.5703125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" style="16" customWidth="1"/>
+    <col min="4" max="7" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C4" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C6" s="20"/>
     </row>
-    <row r="7" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="C7" s="24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C10" s="20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C11" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="C13" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="2:2" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="2:2" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="20" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="20" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="20" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="2:2" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="20" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B46" s="24" t="s">
         <v>25</v>
       </c>
@@ -7998,74 +7998,74 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="90.44140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="7"/>
+    <col min="1" max="1" width="5.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="90.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>125</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="41"/>
     </row>
-    <row r="2" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="136" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="131" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="38"/>
     </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="B5" s="137" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B7" s="137" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B9" s="136" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="135" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A13" s="172" t="s">
+    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="175" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="172"/>
-    </row>
-    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" s="132" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="B13" s="175"/>
+    </row>
+    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:3" s="132" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="140"/>
       <c r="B15" s="138" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="132" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="132" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="140"/>
       <c r="B16" s="139" t="s">
         <v>82</v>
@@ -8074,25 +8074,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="141"/>
       <c r="B17" s="139" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="20" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="141"/>
       <c r="B18" s="139" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="41" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" s="41" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="144"/>
       <c r="B19" s="139" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="132" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="132" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="140"/>
       <c r="B20" s="138" t="s">
         <v>83</v>
@@ -8101,153 +8101,153 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="141"/>
       <c r="B21" s="139" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="142"/>
       <c r="B22" s="143" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="142"/>
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="172" t="s">
+    <row r="24" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="175" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="172"/>
-    </row>
-    <row r="25" spans="1:3" s="8" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B24" s="175"/>
+    </row>
+    <row r="25" spans="1:3" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A25" s="142"/>
       <c r="B25" s="139" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="142"/>
       <c r="B26" s="139"/>
     </row>
-    <row r="27" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="142"/>
       <c r="B27" s="160" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="142"/>
       <c r="B28" s="139" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A29" s="142"/>
       <c r="B29" s="139" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="142"/>
       <c r="B30" s="139"/>
     </row>
-    <row r="31" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="142"/>
       <c r="B31" s="160" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="142"/>
       <c r="B32" s="139" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="142"/>
       <c r="B33" s="139" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="142"/>
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:2" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A35" s="142"/>
       <c r="B35" s="139" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="142"/>
       <c r="B36" s="145" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="142"/>
       <c r="B37" s="10"/>
     </row>
-    <row r="38" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A38" s="172" t="s">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="175" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="172"/>
-    </row>
-    <row r="39" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B38" s="175"/>
+    </row>
+    <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B39" s="139" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:2" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B41" s="139" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:2" s="20" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:2" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="139" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B45" s="139" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="21"/>
     </row>
-    <row r="47" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B47" s="139" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="11"/>
     </row>
-    <row r="49" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="172" t="s">
+    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A49" s="175" t="s">
         <v>8</v>
       </c>
-      <c r="B49" s="172"/>
-    </row>
-    <row r="50" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B49" s="175"/>
+    </row>
+    <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B50" s="139" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B51" s="11"/>
     </row>
-    <row r="52" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A52" s="146" t="s">
         <v>13</v>
       </c>
@@ -8255,7 +8255,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="146" t="s">
         <v>15</v>
       </c>
@@ -8263,7 +8263,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="146" t="s">
         <v>17</v>
       </c>
@@ -8271,19 +8271,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A55" s="135"/>
       <c r="B55" s="139" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A56" s="135"/>
       <c r="B56" s="139" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="146" t="s">
         <v>19</v>
       </c>
@@ -8291,19 +8291,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="135"/>
       <c r="B58" s="139" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="135"/>
       <c r="B59" s="139" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="146" t="s">
         <v>21</v>
       </c>
@@ -8311,13 +8311,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A61" s="135"/>
       <c r="B61" s="139" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A62" s="146" t="s">
         <v>111</v>
       </c>
@@ -8325,36 +8325,36 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="147"/>
       <c r="B63" s="139" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="12"/>
     </row>
-    <row r="65" spans="1:2" s="20" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="172" t="s">
+    <row r="65" spans="1:2" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A65" s="175" t="s">
         <v>11</v>
       </c>
-      <c r="B65" s="172"/>
-    </row>
-    <row r="66" spans="1:2" s="20" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B65" s="175"/>
+    </row>
+    <row r="66" spans="1:2" s="20" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="139" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="13"/>
     </row>
-    <row r="68" spans="1:2" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="172" t="s">
+    <row r="68" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A68" s="175" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="172"/>
-    </row>
-    <row r="69" spans="1:2" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B68" s="175"/>
+    </row>
+    <row r="69" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="154" t="s">
         <v>7</v>
       </c>
@@ -8362,17 +8362,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A70" s="148"/>
       <c r="B70" s="153" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A71" s="148"/>
       <c r="B71" s="149"/>
     </row>
-    <row r="72" spans="1:2" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="154" t="s">
         <v>7</v>
       </c>
@@ -8380,17 +8380,17 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A73" s="148"/>
       <c r="B73" s="153" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A74" s="148"/>
       <c r="B74" s="149"/>
     </row>
-    <row r="75" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="154" t="s">
         <v>7</v>
       </c>
@@ -8398,17 +8398,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="8" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A76" s="148"/>
       <c r="B76" s="137" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A77" s="147"/>
       <c r="B77" s="147"/>
     </row>
-    <row r="78" spans="1:2" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="154" t="s">
         <v>7</v>
       </c>
@@ -8416,17 +8416,17 @@
         <v>126</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A79" s="148"/>
       <c r="B79" s="137" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="1:2" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A80" s="147"/>
       <c r="B80" s="147"/>
     </row>
-    <row r="81" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="154" t="s">
         <v>7</v>
       </c>
@@ -8434,29 +8434,29 @@
         <v>127</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A82" s="148"/>
       <c r="B82" s="152" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A83" s="148"/>
       <c r="B83" s="152" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A84" s="148"/>
       <c r="B84" s="152" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="147"/>
       <c r="B85" s="151"/>
     </row>
-    <row r="86" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="154" t="s">
         <v>7</v>
       </c>
@@ -8464,29 +8464,29 @@
         <v>128</v>
       </c>
     </row>
-    <row r="87" spans="1:2" s="8" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A87" s="148"/>
       <c r="B87" s="137" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A88" s="148"/>
       <c r="B88" s="150" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="1:2" s="8" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A89" s="148"/>
       <c r="B89" s="156" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A90" s="147"/>
       <c r="B90" s="147"/>
     </row>
-    <row r="91" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="154" t="s">
         <v>7</v>
       </c>
@@ -8494,13 +8494,13 @@
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A92" s="135"/>
       <c r="B92" s="152" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="28" t="s">
         <v>56</v>
       </c>
@@ -8536,14 +8536,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="82.109375" style="20" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="5.5703125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="20" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>54</v>
       </c>
@@ -8551,163 +8551,163 @@
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
       <c r="B2" s="45"/>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="42"/>
       <c r="B3" s="35" t="s">
         <v>55</v>
       </c>
       <c r="C3" s="43"/>
     </row>
-    <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="37" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="17"/>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="18" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="17"/>
       <c r="C7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="17" t="s">
         <v>57</v>
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="17"/>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="46.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="17" t="s">
         <v>58</v>
       </c>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="17"/>
       <c r="C11" s="15"/>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="17" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="15"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="17" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:4" ht="30.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="30.75" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="17" t="s">
         <v>61</v>
       </c>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="36" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="19"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>

</xml_diff>

<commit_message>
Added tasks for design
</commit_message>
<xml_diff>
--- a/GANTT chart.xlsx
+++ b/GANTT chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Year2\Fall\CS2043\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\black\Documents\School Stuff\2nd Year\CS 2043\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524AC93F-4617-44D7-8EE8-359F6DF50B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E37FB92E-EF89-4814-AFA2-2F5A0E42AF5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -453,7 +453,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="167">
   <si>
     <t>WBS</t>
   </si>
@@ -1588,6 +1588,30 @@
   </si>
   <si>
     <t>Admin case</t>
+  </si>
+  <si>
+    <t>Elicitation</t>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Requirements Engineering</t>
+  </si>
+  <si>
+    <t>Negotiation</t>
+  </si>
+  <si>
+    <t>Web server</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Interface</t>
   </si>
 </sst>
 </file>
@@ -2948,24 +2972,6 @@
     <xf numFmtId="1" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2973,9 +2979,27 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3027,7 +3051,189 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="25">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3221,13 +3427,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>95250</xdr:colOff>
+          <xdr:colOff>99060</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>106680</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
@@ -3808,29 +4014,29 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN45"/>
+  <dimension ref="A1:BN48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N44" sqref="N44"/>
+      <pane ySplit="7" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="5" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="1.85546875" style="1" customWidth="1"/>
-    <col min="11" max="66" width="2.42578125" style="1" customWidth="1"/>
-    <col min="67" max="16384" width="9.140625" style="3"/>
+    <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.88671875" style="1" customWidth="1"/>
+    <col min="11" max="66" width="2.44140625" style="1" customWidth="1"/>
+    <col min="67" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="123" t="s">
         <v>1</v>
       </c>
@@ -3840,31 +4046,31 @@
       <c r="E1" s="46"/>
       <c r="F1" s="46"/>
       <c r="I1" s="130"/>
-      <c r="K1" s="172" t="s">
+      <c r="K1" s="166" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="172"/>
-      <c r="M1" s="172"/>
-      <c r="N1" s="172"/>
-      <c r="O1" s="172"/>
-      <c r="P1" s="172"/>
-      <c r="Q1" s="172"/>
-      <c r="R1" s="172"/>
-      <c r="S1" s="172"/>
-      <c r="T1" s="172"/>
-      <c r="U1" s="172"/>
-      <c r="V1" s="172"/>
-      <c r="W1" s="172"/>
-      <c r="X1" s="172"/>
-      <c r="Y1" s="172"/>
-      <c r="Z1" s="172"/>
-      <c r="AA1" s="172"/>
-      <c r="AB1" s="172"/>
-      <c r="AC1" s="172"/>
-      <c r="AD1" s="172"/>
-      <c r="AE1" s="172"/>
-    </row>
-    <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
+      <c r="V1" s="166"/>
+      <c r="W1" s="166"/>
+      <c r="X1" s="166"/>
+      <c r="Y1" s="166"/>
+      <c r="Z1" s="166"/>
+      <c r="AA1" s="166"/>
+      <c r="AB1" s="166"/>
+      <c r="AC1" s="166"/>
+      <c r="AD1" s="166"/>
+      <c r="AE1" s="166"/>
+    </row>
+    <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>139</v>
       </c>
@@ -3875,7 +4081,7 @@
       <c r="F2" s="158"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:66" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:66" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="51"/>
       <c r="B3" s="47"/>
       <c r="C3" s="4"/>
@@ -3902,16 +4108,16 @@
       <c r="Z3" s="29"/>
       <c r="AA3" s="29"/>
     </row>
-    <row r="4" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="108"/>
       <c r="B4" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="174">
+      <c r="C4" s="171">
         <v>44151</v>
       </c>
-      <c r="D4" s="174"/>
-      <c r="E4" s="174"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
       <c r="F4" s="109"/>
       <c r="G4" s="112" t="s">
         <v>76</v>
@@ -3921,182 +4127,182 @@
       </c>
       <c r="I4" s="110"/>
       <c r="J4" s="49"/>
-      <c r="K4" s="166" t="str">
+      <c r="K4" s="168" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="167"/>
-      <c r="M4" s="167"/>
-      <c r="N4" s="167"/>
-      <c r="O4" s="167"/>
-      <c r="P4" s="167"/>
-      <c r="Q4" s="168"/>
-      <c r="R4" s="166" t="str">
+      <c r="L4" s="169"/>
+      <c r="M4" s="169"/>
+      <c r="N4" s="169"/>
+      <c r="O4" s="169"/>
+      <c r="P4" s="169"/>
+      <c r="Q4" s="170"/>
+      <c r="R4" s="168" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="167"/>
-      <c r="T4" s="167"/>
-      <c r="U4" s="167"/>
-      <c r="V4" s="167"/>
-      <c r="W4" s="167"/>
-      <c r="X4" s="168"/>
-      <c r="Y4" s="166" t="str">
+      <c r="S4" s="169"/>
+      <c r="T4" s="169"/>
+      <c r="U4" s="169"/>
+      <c r="V4" s="169"/>
+      <c r="W4" s="169"/>
+      <c r="X4" s="170"/>
+      <c r="Y4" s="168" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="167"/>
-      <c r="AA4" s="167"/>
-      <c r="AB4" s="167"/>
-      <c r="AC4" s="167"/>
-      <c r="AD4" s="167"/>
-      <c r="AE4" s="168"/>
-      <c r="AF4" s="166" t="str">
+      <c r="Z4" s="169"/>
+      <c r="AA4" s="169"/>
+      <c r="AB4" s="169"/>
+      <c r="AC4" s="169"/>
+      <c r="AD4" s="169"/>
+      <c r="AE4" s="170"/>
+      <c r="AF4" s="168" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="167"/>
-      <c r="AH4" s="167"/>
-      <c r="AI4" s="167"/>
-      <c r="AJ4" s="167"/>
-      <c r="AK4" s="167"/>
-      <c r="AL4" s="168"/>
-      <c r="AM4" s="166" t="str">
+      <c r="AG4" s="169"/>
+      <c r="AH4" s="169"/>
+      <c r="AI4" s="169"/>
+      <c r="AJ4" s="169"/>
+      <c r="AK4" s="169"/>
+      <c r="AL4" s="170"/>
+      <c r="AM4" s="168" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="167"/>
-      <c r="AO4" s="167"/>
-      <c r="AP4" s="167"/>
-      <c r="AQ4" s="167"/>
-      <c r="AR4" s="167"/>
-      <c r="AS4" s="168"/>
-      <c r="AT4" s="166" t="str">
+      <c r="AN4" s="169"/>
+      <c r="AO4" s="169"/>
+      <c r="AP4" s="169"/>
+      <c r="AQ4" s="169"/>
+      <c r="AR4" s="169"/>
+      <c r="AS4" s="170"/>
+      <c r="AT4" s="168" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="167"/>
-      <c r="AV4" s="167"/>
-      <c r="AW4" s="167"/>
-      <c r="AX4" s="167"/>
-      <c r="AY4" s="167"/>
-      <c r="AZ4" s="168"/>
-      <c r="BA4" s="166" t="str">
+      <c r="AU4" s="169"/>
+      <c r="AV4" s="169"/>
+      <c r="AW4" s="169"/>
+      <c r="AX4" s="169"/>
+      <c r="AY4" s="169"/>
+      <c r="AZ4" s="170"/>
+      <c r="BA4" s="168" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="167"/>
-      <c r="BC4" s="167"/>
-      <c r="BD4" s="167"/>
-      <c r="BE4" s="167"/>
-      <c r="BF4" s="167"/>
-      <c r="BG4" s="168"/>
-      <c r="BH4" s="166" t="str">
+      <c r="BB4" s="169"/>
+      <c r="BC4" s="169"/>
+      <c r="BD4" s="169"/>
+      <c r="BE4" s="169"/>
+      <c r="BF4" s="169"/>
+      <c r="BG4" s="170"/>
+      <c r="BH4" s="168" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="167"/>
-      <c r="BJ4" s="167"/>
-      <c r="BK4" s="167"/>
-      <c r="BL4" s="167"/>
-      <c r="BM4" s="167"/>
-      <c r="BN4" s="168"/>
-    </row>
-    <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BI4" s="169"/>
+      <c r="BJ4" s="169"/>
+      <c r="BK4" s="169"/>
+      <c r="BL4" s="169"/>
+      <c r="BM4" s="169"/>
+      <c r="BN4" s="170"/>
+    </row>
+    <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="108"/>
       <c r="B5" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="173"/>
-      <c r="D5" s="173"/>
-      <c r="E5" s="173"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="167"/>
       <c r="F5" s="111"/>
       <c r="G5" s="111"/>
       <c r="H5" s="111"/>
       <c r="I5" s="111"/>
       <c r="J5" s="49"/>
-      <c r="K5" s="169">
+      <c r="K5" s="172">
         <f>K6</f>
         <v>44151</v>
       </c>
-      <c r="L5" s="170"/>
-      <c r="M5" s="170"/>
-      <c r="N5" s="170"/>
-      <c r="O5" s="170"/>
-      <c r="P5" s="170"/>
-      <c r="Q5" s="171"/>
-      <c r="R5" s="169">
+      <c r="L5" s="173"/>
+      <c r="M5" s="173"/>
+      <c r="N5" s="173"/>
+      <c r="O5" s="173"/>
+      <c r="P5" s="173"/>
+      <c r="Q5" s="174"/>
+      <c r="R5" s="172">
         <f>R6</f>
         <v>44158</v>
       </c>
-      <c r="S5" s="170"/>
-      <c r="T5" s="170"/>
-      <c r="U5" s="170"/>
-      <c r="V5" s="170"/>
-      <c r="W5" s="170"/>
-      <c r="X5" s="171"/>
-      <c r="Y5" s="169">
+      <c r="S5" s="173"/>
+      <c r="T5" s="173"/>
+      <c r="U5" s="173"/>
+      <c r="V5" s="173"/>
+      <c r="W5" s="173"/>
+      <c r="X5" s="174"/>
+      <c r="Y5" s="172">
         <f>Y6</f>
         <v>44165</v>
       </c>
-      <c r="Z5" s="170"/>
-      <c r="AA5" s="170"/>
-      <c r="AB5" s="170"/>
-      <c r="AC5" s="170"/>
-      <c r="AD5" s="170"/>
-      <c r="AE5" s="171"/>
-      <c r="AF5" s="169">
+      <c r="Z5" s="173"/>
+      <c r="AA5" s="173"/>
+      <c r="AB5" s="173"/>
+      <c r="AC5" s="173"/>
+      <c r="AD5" s="173"/>
+      <c r="AE5" s="174"/>
+      <c r="AF5" s="172">
         <f>AF6</f>
         <v>44172</v>
       </c>
-      <c r="AG5" s="170"/>
-      <c r="AH5" s="170"/>
-      <c r="AI5" s="170"/>
-      <c r="AJ5" s="170"/>
-      <c r="AK5" s="170"/>
-      <c r="AL5" s="171"/>
-      <c r="AM5" s="169">
+      <c r="AG5" s="173"/>
+      <c r="AH5" s="173"/>
+      <c r="AI5" s="173"/>
+      <c r="AJ5" s="173"/>
+      <c r="AK5" s="173"/>
+      <c r="AL5" s="174"/>
+      <c r="AM5" s="172">
         <f>AM6</f>
         <v>44179</v>
       </c>
-      <c r="AN5" s="170"/>
-      <c r="AO5" s="170"/>
-      <c r="AP5" s="170"/>
-      <c r="AQ5" s="170"/>
-      <c r="AR5" s="170"/>
-      <c r="AS5" s="171"/>
-      <c r="AT5" s="169">
+      <c r="AN5" s="173"/>
+      <c r="AO5" s="173"/>
+      <c r="AP5" s="173"/>
+      <c r="AQ5" s="173"/>
+      <c r="AR5" s="173"/>
+      <c r="AS5" s="174"/>
+      <c r="AT5" s="172">
         <f>AT6</f>
         <v>44186</v>
       </c>
-      <c r="AU5" s="170"/>
-      <c r="AV5" s="170"/>
-      <c r="AW5" s="170"/>
-      <c r="AX5" s="170"/>
-      <c r="AY5" s="170"/>
-      <c r="AZ5" s="171"/>
-      <c r="BA5" s="169">
+      <c r="AU5" s="173"/>
+      <c r="AV5" s="173"/>
+      <c r="AW5" s="173"/>
+      <c r="AX5" s="173"/>
+      <c r="AY5" s="173"/>
+      <c r="AZ5" s="174"/>
+      <c r="BA5" s="172">
         <f>BA6</f>
         <v>44193</v>
       </c>
-      <c r="BB5" s="170"/>
-      <c r="BC5" s="170"/>
-      <c r="BD5" s="170"/>
-      <c r="BE5" s="170"/>
-      <c r="BF5" s="170"/>
-      <c r="BG5" s="171"/>
-      <c r="BH5" s="169">
+      <c r="BB5" s="173"/>
+      <c r="BC5" s="173"/>
+      <c r="BD5" s="173"/>
+      <c r="BE5" s="173"/>
+      <c r="BF5" s="173"/>
+      <c r="BG5" s="174"/>
+      <c r="BH5" s="172">
         <f>BH6</f>
         <v>44200</v>
       </c>
-      <c r="BI5" s="170"/>
-      <c r="BJ5" s="170"/>
-      <c r="BK5" s="170"/>
-      <c r="BL5" s="170"/>
-      <c r="BM5" s="170"/>
-      <c r="BN5" s="171"/>
-    </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="BI5" s="173"/>
+      <c r="BJ5" s="173"/>
+      <c r="BK5" s="173"/>
+      <c r="BL5" s="173"/>
+      <c r="BM5" s="173"/>
+      <c r="BN5" s="174"/>
+    </row>
+    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" s="48"/>
       <c r="B6" s="49"/>
       <c r="C6" s="49"/>
@@ -4332,7 +4538,7 @@
         <v>44206</v>
       </c>
     </row>
-    <row r="7" spans="1:66" s="122" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" s="122" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="114" t="s">
         <v>0</v>
       </c>
@@ -4586,7 +4792,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="8" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:66" s="54" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="83" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -4665,7 +4871,7 @@
       <c r="BM8" s="105"/>
       <c r="BN8" s="105"/>
     </row>
-    <row r="9" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -4752,7 +4958,7 @@
       <c r="BM9" s="106"/>
       <c r="BN9" s="106"/>
     </row>
-    <row r="10" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.2</v>
@@ -4836,7 +5042,7 @@
       <c r="BM10" s="106"/>
       <c r="BN10" s="106"/>
     </row>
-    <row r="11" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.3</v>
@@ -4920,7 +5126,7 @@
       <c r="BM11" s="106"/>
       <c r="BN11" s="106"/>
     </row>
-    <row r="12" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.1</v>
@@ -5004,7 +5210,7 @@
       <c r="BM12" s="106"/>
       <c r="BN12" s="106"/>
     </row>
-    <row r="13" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.2</v>
@@ -5088,7 +5294,7 @@
       <c r="BM13" s="106"/>
       <c r="BN13" s="106"/>
     </row>
-    <row r="14" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.3.3</v>
@@ -5172,7 +5378,7 @@
       <c r="BM14" s="106"/>
       <c r="BN14" s="106"/>
     </row>
-    <row r="15" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.4</v>
@@ -5256,7 +5462,7 @@
       <c r="BM15" s="106"/>
       <c r="BN15" s="106"/>
     </row>
-    <row r="16" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.5</v>
@@ -5340,7 +5546,7 @@
       <c r="BM16" s="106"/>
       <c r="BN16" s="106"/>
     </row>
-    <row r="17" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A17" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.6</v>
@@ -5424,7 +5630,7 @@
       <c r="BM17" s="106"/>
       <c r="BN17" s="106"/>
     </row>
-    <row r="18" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:66" s="54" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -5502,7 +5708,7 @@
       <c r="BM18" s="107"/>
       <c r="BN18" s="107"/>
     </row>
-    <row r="19" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:66" s="60" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A19" s="59" t="str">
         <f t="shared" ref="A19:A24" si="6">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
@@ -5586,7 +5792,7 @@
       <c r="BM19" s="106"/>
       <c r="BN19" s="106"/>
     </row>
-    <row r="20" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="59" t="str">
         <f t="shared" si="6"/>
         <v>2.2</v>
@@ -5670,7 +5876,7 @@
       <c r="BM20" s="106"/>
       <c r="BN20" s="106"/>
     </row>
-    <row r="21" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A21" s="59" t="str">
         <f t="shared" si="6"/>
         <v>2.3</v>
@@ -5754,7 +5960,7 @@
       <c r="BM21" s="106"/>
       <c r="BN21" s="106"/>
     </row>
-    <row r="22" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="str">
         <f t="shared" si="6"/>
         <v>2.4</v>
@@ -5838,7 +6044,7 @@
       <c r="BM22" s="106"/>
       <c r="BN22" s="106"/>
     </row>
-    <row r="23" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A23" s="59" t="str">
         <f t="shared" si="6"/>
         <v>2.5</v>
@@ -5922,7 +6128,7 @@
       <c r="BM23" s="106"/>
       <c r="BN23" s="106"/>
     </row>
-    <row r="24" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A24" s="59" t="str">
         <f t="shared" si="6"/>
         <v>2.6</v>
@@ -6005,7 +6211,7 @@
       <c r="BM24" s="106"/>
       <c r="BN24" s="106"/>
     </row>
-    <row r="25" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:66" s="54" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A25" s="52" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
@@ -6016,13 +6222,13 @@
       <c r="D25" s="55"/>
       <c r="E25" s="101"/>
       <c r="F25" s="101" t="str">
-        <f t="shared" ref="F25:F35" si="7">IF(ISBLANK(E25)," - ",IF(G25=0,E25,E25+G25-1))</f>
+        <f t="shared" ref="F25:F38" si="7">IF(ISBLANK(E25)," - ",IF(G25=0,E25,E25+G25-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G25" s="56"/>
       <c r="H25" s="57"/>
       <c r="I25" s="58" t="str">
-        <f t="shared" ref="I25:I38" si="8">IF(OR(F25=0,E25=0)," - ",NETWORKDAYS(E25,F25))</f>
+        <f t="shared" ref="I25:I41" si="8">IF(OR(F25=0,E25=0)," - ",NETWORKDAYS(E25,F25))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J25" s="95"/>
@@ -6083,31 +6289,31 @@
       <c r="BM25" s="107"/>
       <c r="BN25" s="107"/>
     </row>
-    <row r="26" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:66" s="60" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A26" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
       </c>
       <c r="B26" s="124" t="s">
-        <v>9</v>
+        <v>162</v>
       </c>
       <c r="D26" s="125"/>
       <c r="E26" s="99">
-        <v>44157</v>
+        <v>44166</v>
       </c>
       <c r="F26" s="100">
         <f t="shared" si="7"/>
-        <v>44159</v>
+        <v>44174</v>
       </c>
       <c r="G26" s="61">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H26" s="62">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I26" s="63">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J26" s="94"/>
       <c r="K26" s="106"/>
@@ -6167,27 +6373,27 @@
       <c r="BM26" s="106"/>
       <c r="BN26" s="106"/>
     </row>
-    <row r="27" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.2</v>
-      </c>
-      <c r="B27" s="124" t="s">
-        <v>9</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>3.1.1</v>
+      </c>
+      <c r="B27" s="126" t="s">
+        <v>159</v>
       </c>
       <c r="D27" s="125"/>
       <c r="E27" s="99">
-        <v>44158</v>
+        <v>44166</v>
       </c>
       <c r="F27" s="100">
         <f t="shared" si="7"/>
-        <v>44159</v>
+        <v>44167</v>
       </c>
       <c r="G27" s="61">
         <v>2</v>
       </c>
       <c r="H27" s="62">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I27" s="63">
         <f t="shared" si="8"/>
@@ -6251,31 +6457,31 @@
       <c r="BM27" s="106"/>
       <c r="BN27" s="106"/>
     </row>
-    <row r="28" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A28" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.3</v>
-      </c>
-      <c r="B28" s="124" t="s">
-        <v>9</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>3.1.2</v>
+      </c>
+      <c r="B28" s="126" t="s">
+        <v>160</v>
       </c>
       <c r="D28" s="125"/>
       <c r="E28" s="99">
-        <v>44159</v>
+        <v>44167</v>
       </c>
       <c r="F28" s="100">
         <f t="shared" si="7"/>
-        <v>44161</v>
+        <v>44168</v>
       </c>
       <c r="G28" s="61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H28" s="62">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I28" s="63">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J28" s="94"/>
       <c r="K28" s="106"/>
@@ -6335,31 +6541,31 @@
       <c r="BM28" s="106"/>
       <c r="BN28" s="106"/>
     </row>
-    <row r="29" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A29" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.4</v>
-      </c>
-      <c r="B29" s="124" t="s">
-        <v>9</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>3.1.3</v>
+      </c>
+      <c r="B29" s="126" t="s">
+        <v>161</v>
       </c>
       <c r="D29" s="125"/>
       <c r="E29" s="99">
-        <v>44160</v>
+        <v>44168</v>
       </c>
       <c r="F29" s="100">
         <f t="shared" si="7"/>
-        <v>44162</v>
+        <v>44169</v>
       </c>
       <c r="G29" s="61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H29" s="62">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I29" s="63">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J29" s="94"/>
       <c r="K29" s="106"/>
@@ -6419,31 +6625,31 @@
       <c r="BM29" s="106"/>
       <c r="BN29" s="106"/>
     </row>
-    <row r="30" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A30" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.5</v>
-      </c>
-      <c r="B30" s="124" t="s">
-        <v>9</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>3.1.4</v>
+      </c>
+      <c r="B30" s="126" t="s">
+        <v>163</v>
       </c>
       <c r="D30" s="125"/>
       <c r="E30" s="99">
-        <v>44161</v>
+        <v>44169</v>
       </c>
       <c r="F30" s="100">
         <f t="shared" si="7"/>
-        <v>44164</v>
+        <v>44170</v>
       </c>
       <c r="G30" s="61">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H30" s="62">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I30" s="63">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J30" s="94"/>
       <c r="K30" s="106"/>
@@ -6503,109 +6709,115 @@
       <c r="BM30" s="106"/>
       <c r="BN30" s="106"/>
     </row>
-    <row r="31" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="52" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>4</v>
-      </c>
-      <c r="B31" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="D31" s="55"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="101" t="str">
+    <row r="31" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A31" s="59" t="str">
+        <f t="shared" ref="A31:A33" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>3.2</v>
+      </c>
+      <c r="B31" s="124" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="125"/>
+      <c r="E31" s="99">
+        <v>44167</v>
+      </c>
+      <c r="F31" s="100">
         <f t="shared" si="7"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G31" s="56"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="58" t="str">
+        <v>44169</v>
+      </c>
+      <c r="G31" s="61">
+        <v>3</v>
+      </c>
+      <c r="H31" s="62">
+        <v>1</v>
+      </c>
+      <c r="I31" s="63">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J31" s="95"/>
-      <c r="K31" s="107"/>
-      <c r="L31" s="107"/>
-      <c r="M31" s="107"/>
-      <c r="N31" s="107"/>
-      <c r="O31" s="107"/>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
-      <c r="S31" s="107"/>
-      <c r="T31" s="107"/>
-      <c r="U31" s="107"/>
-      <c r="V31" s="107"/>
-      <c r="W31" s="107"/>
-      <c r="X31" s="107"/>
-      <c r="Y31" s="107"/>
-      <c r="Z31" s="107"/>
-      <c r="AA31" s="107"/>
-      <c r="AB31" s="107"/>
-      <c r="AC31" s="107"/>
-      <c r="AD31" s="107"/>
-      <c r="AE31" s="107"/>
-      <c r="AF31" s="107"/>
-      <c r="AG31" s="107"/>
-      <c r="AH31" s="107"/>
-      <c r="AI31" s="107"/>
-      <c r="AJ31" s="107"/>
-      <c r="AK31" s="107"/>
-      <c r="AL31" s="107"/>
-      <c r="AM31" s="107"/>
-      <c r="AN31" s="107"/>
-      <c r="AO31" s="107"/>
-      <c r="AP31" s="107"/>
-      <c r="AQ31" s="107"/>
-      <c r="AR31" s="107"/>
-      <c r="AS31" s="107"/>
-      <c r="AT31" s="107"/>
-      <c r="AU31" s="107"/>
-      <c r="AV31" s="107"/>
-      <c r="AW31" s="107"/>
-      <c r="AX31" s="107"/>
-      <c r="AY31" s="107"/>
-      <c r="AZ31" s="107"/>
-      <c r="BA31" s="107"/>
-      <c r="BB31" s="107"/>
-      <c r="BC31" s="107"/>
-      <c r="BD31" s="107"/>
-      <c r="BE31" s="107"/>
-      <c r="BF31" s="107"/>
-      <c r="BG31" s="107"/>
-      <c r="BH31" s="107"/>
-      <c r="BI31" s="107"/>
-      <c r="BJ31" s="107"/>
-      <c r="BK31" s="107"/>
-      <c r="BL31" s="107"/>
-      <c r="BM31" s="107"/>
-      <c r="BN31" s="107"/>
-    </row>
-    <row r="32" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="J31" s="94"/>
+      <c r="K31" s="106"/>
+      <c r="L31" s="106"/>
+      <c r="M31" s="106"/>
+      <c r="N31" s="106"/>
+      <c r="O31" s="106"/>
+      <c r="P31" s="106"/>
+      <c r="Q31" s="106"/>
+      <c r="R31" s="106"/>
+      <c r="S31" s="106"/>
+      <c r="T31" s="106"/>
+      <c r="U31" s="106"/>
+      <c r="V31" s="106"/>
+      <c r="W31" s="106"/>
+      <c r="X31" s="106"/>
+      <c r="Y31" s="106"/>
+      <c r="Z31" s="106"/>
+      <c r="AA31" s="106"/>
+      <c r="AB31" s="106"/>
+      <c r="AC31" s="106"/>
+      <c r="AD31" s="106"/>
+      <c r="AE31" s="106"/>
+      <c r="AF31" s="106"/>
+      <c r="AG31" s="106"/>
+      <c r="AH31" s="106"/>
+      <c r="AI31" s="106"/>
+      <c r="AJ31" s="106"/>
+      <c r="AK31" s="106"/>
+      <c r="AL31" s="106"/>
+      <c r="AM31" s="106"/>
+      <c r="AN31" s="106"/>
+      <c r="AO31" s="106"/>
+      <c r="AP31" s="106"/>
+      <c r="AQ31" s="106"/>
+      <c r="AR31" s="106"/>
+      <c r="AS31" s="106"/>
+      <c r="AT31" s="106"/>
+      <c r="AU31" s="106"/>
+      <c r="AV31" s="106"/>
+      <c r="AW31" s="106"/>
+      <c r="AX31" s="106"/>
+      <c r="AY31" s="106"/>
+      <c r="AZ31" s="106"/>
+      <c r="BA31" s="106"/>
+      <c r="BB31" s="106"/>
+      <c r="BC31" s="106"/>
+      <c r="BD31" s="106"/>
+      <c r="BE31" s="106"/>
+      <c r="BF31" s="106"/>
+      <c r="BG31" s="106"/>
+      <c r="BH31" s="106"/>
+      <c r="BI31" s="106"/>
+      <c r="BJ31" s="106"/>
+      <c r="BK31" s="106"/>
+      <c r="BL31" s="106"/>
+      <c r="BM31" s="106"/>
+      <c r="BN31" s="106"/>
+    </row>
+    <row r="32" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A32" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.1</v>
+        <f t="shared" si="9"/>
+        <v>3.3</v>
       </c>
       <c r="B32" s="124" t="s">
-        <v>9</v>
+        <v>165</v>
       </c>
       <c r="D32" s="125"/>
       <c r="E32" s="99">
         <v>44167</v>
       </c>
       <c r="F32" s="100">
-        <f>IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
-        <v>44167</v>
+        <f t="shared" ref="F32" si="10">IF(ISBLANK(E32)," - ",IF(G32=0,E32,E32+G32-1))</f>
+        <v>44171</v>
       </c>
       <c r="G32" s="61">
+        <v>5</v>
+      </c>
+      <c r="H32" s="62">
         <v>1</v>
       </c>
-      <c r="H32" s="62">
-        <v>0</v>
-      </c>
       <c r="I32" s="63">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" ref="I32" si="11">IF(OR(F32=0,E32=0)," - ",NETWORKDAYS(E32,F32))</f>
+        <v>3</v>
       </c>
       <c r="J32" s="94"/>
       <c r="K32" s="106"/>
@@ -6665,31 +6877,31 @@
       <c r="BM32" s="106"/>
       <c r="BN32" s="106"/>
     </row>
-    <row r="33" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A33" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.2</v>
+        <f t="shared" si="9"/>
+        <v>3.4</v>
       </c>
       <c r="B33" s="124" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D33" s="125"/>
       <c r="E33" s="99">
-        <v>44168</v>
+        <v>44167</v>
       </c>
       <c r="F33" s="100">
-        <f t="shared" si="7"/>
-        <v>44168</v>
+        <f t="shared" ref="F33" si="12">IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
+        <v>44170</v>
       </c>
       <c r="G33" s="61">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H33" s="62">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I33" s="63">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" ref="I33" si="13">IF(OR(F33=0,E33=0)," - ",NETWORKDAYS(E33,F33))</f>
+        <v>3</v>
       </c>
       <c r="J33" s="94"/>
       <c r="K33" s="106"/>
@@ -6749,115 +6961,109 @@
       <c r="BM33" s="106"/>
       <c r="BN33" s="106"/>
     </row>
-    <row r="34" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="59" t="str">
+    <row r="34" spans="1:66" s="54" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A34" s="52" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>4</v>
+      </c>
+      <c r="B34" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="55"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G34" s="56"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="58" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J34" s="95"/>
+      <c r="K34" s="107"/>
+      <c r="L34" s="107"/>
+      <c r="M34" s="107"/>
+      <c r="N34" s="107"/>
+      <c r="O34" s="107"/>
+      <c r="P34" s="107"/>
+      <c r="Q34" s="107"/>
+      <c r="R34" s="107"/>
+      <c r="S34" s="107"/>
+      <c r="T34" s="107"/>
+      <c r="U34" s="107"/>
+      <c r="V34" s="107"/>
+      <c r="W34" s="107"/>
+      <c r="X34" s="107"/>
+      <c r="Y34" s="107"/>
+      <c r="Z34" s="107"/>
+      <c r="AA34" s="107"/>
+      <c r="AB34" s="107"/>
+      <c r="AC34" s="107"/>
+      <c r="AD34" s="107"/>
+      <c r="AE34" s="107"/>
+      <c r="AF34" s="107"/>
+      <c r="AG34" s="107"/>
+      <c r="AH34" s="107"/>
+      <c r="AI34" s="107"/>
+      <c r="AJ34" s="107"/>
+      <c r="AK34" s="107"/>
+      <c r="AL34" s="107"/>
+      <c r="AM34" s="107"/>
+      <c r="AN34" s="107"/>
+      <c r="AO34" s="107"/>
+      <c r="AP34" s="107"/>
+      <c r="AQ34" s="107"/>
+      <c r="AR34" s="107"/>
+      <c r="AS34" s="107"/>
+      <c r="AT34" s="107"/>
+      <c r="AU34" s="107"/>
+      <c r="AV34" s="107"/>
+      <c r="AW34" s="107"/>
+      <c r="AX34" s="107"/>
+      <c r="AY34" s="107"/>
+      <c r="AZ34" s="107"/>
+      <c r="BA34" s="107"/>
+      <c r="BB34" s="107"/>
+      <c r="BC34" s="107"/>
+      <c r="BD34" s="107"/>
+      <c r="BE34" s="107"/>
+      <c r="BF34" s="107"/>
+      <c r="BG34" s="107"/>
+      <c r="BH34" s="107"/>
+      <c r="BI34" s="107"/>
+      <c r="BJ34" s="107"/>
+      <c r="BK34" s="107"/>
+      <c r="BL34" s="107"/>
+      <c r="BM34" s="107"/>
+      <c r="BN34" s="107"/>
+    </row>
+    <row r="35" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A35" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.3</v>
-      </c>
-      <c r="B34" s="124" t="s">
+        <v>4.1</v>
+      </c>
+      <c r="B35" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="125"/>
-      <c r="E34" s="99">
-        <v>44169</v>
-      </c>
-      <c r="F34" s="100">
-        <f t="shared" si="7"/>
-        <v>44169</v>
-      </c>
-      <c r="G34" s="61">
+      <c r="D35" s="125"/>
+      <c r="E35" s="99">
+        <v>44167</v>
+      </c>
+      <c r="F35" s="100">
+        <f>IF(ISBLANK(E35)," - ",IF(G35=0,E35,E35+G35-1))</f>
+        <v>44167</v>
+      </c>
+      <c r="G35" s="61">
         <v>1</v>
       </c>
-      <c r="H34" s="62">
+      <c r="H35" s="62">
         <v>0</v>
       </c>
-      <c r="I34" s="63">
+      <c r="I35" s="63">
         <f t="shared" si="8"/>
         <v>1</v>
-      </c>
-      <c r="J34" s="94"/>
-      <c r="K34" s="106"/>
-      <c r="L34" s="106"/>
-      <c r="M34" s="106"/>
-      <c r="N34" s="106"/>
-      <c r="O34" s="106"/>
-      <c r="P34" s="106"/>
-      <c r="Q34" s="106"/>
-      <c r="R34" s="106"/>
-      <c r="S34" s="106"/>
-      <c r="T34" s="106"/>
-      <c r="U34" s="106"/>
-      <c r="V34" s="106"/>
-      <c r="W34" s="106"/>
-      <c r="X34" s="106"/>
-      <c r="Y34" s="106"/>
-      <c r="Z34" s="106"/>
-      <c r="AA34" s="106"/>
-      <c r="AB34" s="106"/>
-      <c r="AC34" s="106"/>
-      <c r="AD34" s="106"/>
-      <c r="AE34" s="106"/>
-      <c r="AF34" s="106"/>
-      <c r="AG34" s="106"/>
-      <c r="AH34" s="106"/>
-      <c r="AI34" s="106"/>
-      <c r="AJ34" s="106"/>
-      <c r="AK34" s="106"/>
-      <c r="AL34" s="106"/>
-      <c r="AM34" s="106"/>
-      <c r="AN34" s="106"/>
-      <c r="AO34" s="106"/>
-      <c r="AP34" s="106"/>
-      <c r="AQ34" s="106"/>
-      <c r="AR34" s="106"/>
-      <c r="AS34" s="106"/>
-      <c r="AT34" s="106"/>
-      <c r="AU34" s="106"/>
-      <c r="AV34" s="106"/>
-      <c r="AW34" s="106"/>
-      <c r="AX34" s="106"/>
-      <c r="AY34" s="106"/>
-      <c r="AZ34" s="106"/>
-      <c r="BA34" s="106"/>
-      <c r="BB34" s="106"/>
-      <c r="BC34" s="106"/>
-      <c r="BD34" s="106"/>
-      <c r="BE34" s="106"/>
-      <c r="BF34" s="106"/>
-      <c r="BG34" s="106"/>
-      <c r="BH34" s="106"/>
-      <c r="BI34" s="106"/>
-      <c r="BJ34" s="106"/>
-      <c r="BK34" s="106"/>
-      <c r="BL34" s="106"/>
-      <c r="BM34" s="106"/>
-      <c r="BN34" s="106"/>
-    </row>
-    <row r="35" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.4</v>
-      </c>
-      <c r="B35" s="124" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="125"/>
-      <c r="E35" s="99">
-        <v>44170</v>
-      </c>
-      <c r="F35" s="100">
-        <f t="shared" si="7"/>
-        <v>44170</v>
-      </c>
-      <c r="G35" s="61">
-        <v>1</v>
-      </c>
-      <c r="H35" s="62">
-        <v>0</v>
-      </c>
-      <c r="I35" s="63">
-        <f t="shared" si="8"/>
-        <v>0</v>
       </c>
       <c r="J35" s="94"/>
       <c r="K35" s="106"/>
@@ -6917,21 +7123,21 @@
       <c r="BM35" s="106"/>
       <c r="BN35" s="106"/>
     </row>
-    <row r="36" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A36" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="B36" s="124" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="125"/>
       <c r="E36" s="99">
-        <v>44170</v>
+        <v>44168</v>
       </c>
       <c r="F36" s="100">
-        <f>IF(ISBLANK(E36)," - ",IF(G36=0,E36,E36+G36-1))</f>
-        <v>44170</v>
+        <f t="shared" si="7"/>
+        <v>44168</v>
       </c>
       <c r="G36" s="61">
         <v>1</v>
@@ -6941,7 +7147,7 @@
       </c>
       <c r="I36" s="63">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" s="94"/>
       <c r="K36" s="106"/>
@@ -7001,20 +7207,33 @@
       <c r="BM36" s="106"/>
       <c r="BN36" s="106"/>
     </row>
-    <row r="37" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="59"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="102"/>
-      <c r="F37" s="102"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="67"/>
-      <c r="I37" s="68" t="str">
+    <row r="37" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A37" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.3</v>
+      </c>
+      <c r="B37" s="124" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="125"/>
+      <c r="E37" s="99">
+        <v>44169</v>
+      </c>
+      <c r="F37" s="100">
+        <f t="shared" si="7"/>
+        <v>44169</v>
+      </c>
+      <c r="G37" s="61">
+        <v>1</v>
+      </c>
+      <c r="H37" s="62">
+        <v>0</v>
+      </c>
+      <c r="I37" s="63">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J37" s="96"/>
+        <v>1</v>
+      </c>
+      <c r="J37" s="94"/>
       <c r="K37" s="106"/>
       <c r="L37" s="106"/>
       <c r="M37" s="106"/>
@@ -7072,20 +7291,33 @@
       <c r="BM37" s="106"/>
       <c r="BN37" s="106"/>
     </row>
-    <row r="38" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="59"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="102"/>
-      <c r="F38" s="102"/>
-      <c r="G38" s="66"/>
-      <c r="H38" s="67"/>
-      <c r="I38" s="68" t="str">
+    <row r="38" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A38" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.4</v>
+      </c>
+      <c r="B38" s="124" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="125"/>
+      <c r="E38" s="99">
+        <v>44170</v>
+      </c>
+      <c r="F38" s="100">
+        <f t="shared" si="7"/>
+        <v>44170</v>
+      </c>
+      <c r="G38" s="61">
+        <v>1</v>
+      </c>
+      <c r="H38" s="62">
+        <v>0</v>
+      </c>
+      <c r="I38" s="63">
         <f t="shared" si="8"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J38" s="96"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="94"/>
       <c r="K38" s="106"/>
       <c r="L38" s="106"/>
       <c r="M38" s="106"/>
@@ -7143,19 +7375,33 @@
       <c r="BM38" s="106"/>
       <c r="BN38" s="106"/>
     </row>
-    <row r="39" spans="1:66" s="74" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="70" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="71"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="103"/>
-      <c r="F39" s="103"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
-      <c r="J39" s="97"/>
+    <row r="39" spans="1:66" s="60" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A39" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.5</v>
+      </c>
+      <c r="B39" s="124" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="125"/>
+      <c r="E39" s="99">
+        <v>44170</v>
+      </c>
+      <c r="F39" s="100">
+        <f>IF(ISBLANK(E39)," - ",IF(G39=0,E39,E39+G39-1))</f>
+        <v>44170</v>
+      </c>
+      <c r="G39" s="61">
+        <v>1</v>
+      </c>
+      <c r="H39" s="62">
+        <v>0</v>
+      </c>
+      <c r="I39" s="63">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="94"/>
       <c r="K39" s="106"/>
       <c r="L39" s="106"/>
       <c r="M39" s="106"/>
@@ -7213,19 +7459,20 @@
       <c r="BM39" s="106"/>
       <c r="BN39" s="106"/>
     </row>
-    <row r="40" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="75" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="76"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="104"/>
-      <c r="F40" s="104"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="76"/>
-      <c r="J40" s="97"/>
+    <row r="40" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A40" s="59"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="102"/>
+      <c r="F40" s="102"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="68" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J40" s="96"/>
       <c r="K40" s="106"/>
       <c r="L40" s="106"/>
       <c r="M40" s="106"/>
@@ -7283,28 +7530,20 @@
       <c r="BM40" s="106"/>
       <c r="BN40" s="106"/>
     </row>
-    <row r="41" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="128" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>1</v>
-      </c>
-      <c r="B41" s="129" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="77"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="99"/>
-      <c r="F41" s="100" t="str">
-        <f t="shared" ref="F41:F44" si="9">IF(ISBLANK(E41)," - ",IF(G41=0,E41,E41+G41-1))</f>
+    <row r="41" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A41" s="59"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="102"/>
+      <c r="F41" s="102"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="68" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G41" s="61"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="79" t="str">
-        <f>IF(OR(F41=0,E41=0)," - ",NETWORKDAYS(E41,F41))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J41" s="98"/>
+      <c r="J41" s="96"/>
       <c r="K41" s="106"/>
       <c r="L41" s="106"/>
       <c r="M41" s="106"/>
@@ -7362,28 +7601,19 @@
       <c r="BM41" s="106"/>
       <c r="BN41" s="106"/>
     </row>
-    <row r="42" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>1.1</v>
-      </c>
-      <c r="B42" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="80"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="99"/>
-      <c r="F42" s="100" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G42" s="61"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="79" t="str">
-        <f t="shared" ref="I42:I44" si="10">IF(OR(F42=0,E42=0)," - ",NETWORKDAYS(E42,F42))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J42" s="98"/>
+    <row r="42" spans="1:66" s="74" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A42" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="71"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
+      <c r="E42" s="103"/>
+      <c r="F42" s="103"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="97"/>
       <c r="K42" s="106"/>
       <c r="L42" s="106"/>
       <c r="M42" s="106"/>
@@ -7441,28 +7671,19 @@
       <c r="BM42" s="106"/>
       <c r="BN42" s="106"/>
     </row>
-    <row r="43" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A43" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.1.1</v>
-      </c>
-      <c r="B43" s="81" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="80"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="99"/>
-      <c r="F43" s="100" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G43" s="61"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="79" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J43" s="98"/>
+    <row r="43" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A43" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="76"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="104"/>
+      <c r="F43" s="104"/>
+      <c r="G43" s="76"/>
+      <c r="H43" s="76"/>
+      <c r="I43" s="76"/>
+      <c r="J43" s="97"/>
       <c r="K43" s="106"/>
       <c r="L43" s="106"/>
       <c r="M43" s="106"/>
@@ -7520,25 +7741,25 @@
       <c r="BM43" s="106"/>
       <c r="BN43" s="106"/>
     </row>
-    <row r="44" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A44" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
-        <v>1.1.1.1</v>
-      </c>
-      <c r="B44" s="81" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="80"/>
+    <row r="44" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A44" s="128" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>1</v>
+      </c>
+      <c r="B44" s="129" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="77"/>
       <c r="D44" s="78"/>
       <c r="E44" s="99"/>
       <c r="F44" s="100" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="F44:F47" si="14">IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G44" s="61"/>
       <c r="H44" s="62"/>
       <c r="I44" s="79" t="str">
-        <f t="shared" si="10"/>
+        <f>IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J44" s="98"/>
@@ -7599,89 +7820,317 @@
       <c r="BM44" s="106"/>
       <c r="BN44" s="106"/>
     </row>
-    <row r="45" spans="1:66" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="161" t="str">
+    <row r="45" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A45" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>1.1</v>
+      </c>
+      <c r="B45" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="80"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="99"/>
+      <c r="F45" s="100" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G45" s="61"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="79" t="str">
+        <f t="shared" ref="I45:I47" si="15">IF(OR(F45=0,E45=0)," - ",NETWORKDAYS(E45,F45))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J45" s="98"/>
+      <c r="K45" s="106"/>
+      <c r="L45" s="106"/>
+      <c r="M45" s="106"/>
+      <c r="N45" s="106"/>
+      <c r="O45" s="106"/>
+      <c r="P45" s="106"/>
+      <c r="Q45" s="106"/>
+      <c r="R45" s="106"/>
+      <c r="S45" s="106"/>
+      <c r="T45" s="106"/>
+      <c r="U45" s="106"/>
+      <c r="V45" s="106"/>
+      <c r="W45" s="106"/>
+      <c r="X45" s="106"/>
+      <c r="Y45" s="106"/>
+      <c r="Z45" s="106"/>
+      <c r="AA45" s="106"/>
+      <c r="AB45" s="106"/>
+      <c r="AC45" s="106"/>
+      <c r="AD45" s="106"/>
+      <c r="AE45" s="106"/>
+      <c r="AF45" s="106"/>
+      <c r="AG45" s="106"/>
+      <c r="AH45" s="106"/>
+      <c r="AI45" s="106"/>
+      <c r="AJ45" s="106"/>
+      <c r="AK45" s="106"/>
+      <c r="AL45" s="106"/>
+      <c r="AM45" s="106"/>
+      <c r="AN45" s="106"/>
+      <c r="AO45" s="106"/>
+      <c r="AP45" s="106"/>
+      <c r="AQ45" s="106"/>
+      <c r="AR45" s="106"/>
+      <c r="AS45" s="106"/>
+      <c r="AT45" s="106"/>
+      <c r="AU45" s="106"/>
+      <c r="AV45" s="106"/>
+      <c r="AW45" s="106"/>
+      <c r="AX45" s="106"/>
+      <c r="AY45" s="106"/>
+      <c r="AZ45" s="106"/>
+      <c r="BA45" s="106"/>
+      <c r="BB45" s="106"/>
+      <c r="BC45" s="106"/>
+      <c r="BD45" s="106"/>
+      <c r="BE45" s="106"/>
+      <c r="BF45" s="106"/>
+      <c r="BG45" s="106"/>
+      <c r="BH45" s="106"/>
+      <c r="BI45" s="106"/>
+      <c r="BJ45" s="106"/>
+      <c r="BK45" s="106"/>
+      <c r="BL45" s="106"/>
+      <c r="BM45" s="106"/>
+      <c r="BN45" s="106"/>
+    </row>
+    <row r="46" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A46" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>1.1.1</v>
+      </c>
+      <c r="B46" s="81" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="80"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="99"/>
+      <c r="F46" s="100" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G46" s="61"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="79" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J46" s="98"/>
+      <c r="K46" s="106"/>
+      <c r="L46" s="106"/>
+      <c r="M46" s="106"/>
+      <c r="N46" s="106"/>
+      <c r="O46" s="106"/>
+      <c r="P46" s="106"/>
+      <c r="Q46" s="106"/>
+      <c r="R46" s="106"/>
+      <c r="S46" s="106"/>
+      <c r="T46" s="106"/>
+      <c r="U46" s="106"/>
+      <c r="V46" s="106"/>
+      <c r="W46" s="106"/>
+      <c r="X46" s="106"/>
+      <c r="Y46" s="106"/>
+      <c r="Z46" s="106"/>
+      <c r="AA46" s="106"/>
+      <c r="AB46" s="106"/>
+      <c r="AC46" s="106"/>
+      <c r="AD46" s="106"/>
+      <c r="AE46" s="106"/>
+      <c r="AF46" s="106"/>
+      <c r="AG46" s="106"/>
+      <c r="AH46" s="106"/>
+      <c r="AI46" s="106"/>
+      <c r="AJ46" s="106"/>
+      <c r="AK46" s="106"/>
+      <c r="AL46" s="106"/>
+      <c r="AM46" s="106"/>
+      <c r="AN46" s="106"/>
+      <c r="AO46" s="106"/>
+      <c r="AP46" s="106"/>
+      <c r="AQ46" s="106"/>
+      <c r="AR46" s="106"/>
+      <c r="AS46" s="106"/>
+      <c r="AT46" s="106"/>
+      <c r="AU46" s="106"/>
+      <c r="AV46" s="106"/>
+      <c r="AW46" s="106"/>
+      <c r="AX46" s="106"/>
+      <c r="AY46" s="106"/>
+      <c r="AZ46" s="106"/>
+      <c r="BA46" s="106"/>
+      <c r="BB46" s="106"/>
+      <c r="BC46" s="106"/>
+      <c r="BD46" s="106"/>
+      <c r="BE46" s="106"/>
+      <c r="BF46" s="106"/>
+      <c r="BG46" s="106"/>
+      <c r="BH46" s="106"/>
+      <c r="BI46" s="106"/>
+      <c r="BJ46" s="106"/>
+      <c r="BK46" s="106"/>
+      <c r="BL46" s="106"/>
+      <c r="BM46" s="106"/>
+      <c r="BN46" s="106"/>
+    </row>
+    <row r="47" spans="1:66" s="69" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A47" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="B47" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="80"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="99"/>
+      <c r="F47" s="100" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G47" s="61"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="79" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J47" s="98"/>
+      <c r="K47" s="106"/>
+      <c r="L47" s="106"/>
+      <c r="M47" s="106"/>
+      <c r="N47" s="106"/>
+      <c r="O47" s="106"/>
+      <c r="P47" s="106"/>
+      <c r="Q47" s="106"/>
+      <c r="R47" s="106"/>
+      <c r="S47" s="106"/>
+      <c r="T47" s="106"/>
+      <c r="U47" s="106"/>
+      <c r="V47" s="106"/>
+      <c r="W47" s="106"/>
+      <c r="X47" s="106"/>
+      <c r="Y47" s="106"/>
+      <c r="Z47" s="106"/>
+      <c r="AA47" s="106"/>
+      <c r="AB47" s="106"/>
+      <c r="AC47" s="106"/>
+      <c r="AD47" s="106"/>
+      <c r="AE47" s="106"/>
+      <c r="AF47" s="106"/>
+      <c r="AG47" s="106"/>
+      <c r="AH47" s="106"/>
+      <c r="AI47" s="106"/>
+      <c r="AJ47" s="106"/>
+      <c r="AK47" s="106"/>
+      <c r="AL47" s="106"/>
+      <c r="AM47" s="106"/>
+      <c r="AN47" s="106"/>
+      <c r="AO47" s="106"/>
+      <c r="AP47" s="106"/>
+      <c r="AQ47" s="106"/>
+      <c r="AR47" s="106"/>
+      <c r="AS47" s="106"/>
+      <c r="AT47" s="106"/>
+      <c r="AU47" s="106"/>
+      <c r="AV47" s="106"/>
+      <c r="AW47" s="106"/>
+      <c r="AX47" s="106"/>
+      <c r="AY47" s="106"/>
+      <c r="AZ47" s="106"/>
+      <c r="BA47" s="106"/>
+      <c r="BB47" s="106"/>
+      <c r="BC47" s="106"/>
+      <c r="BD47" s="106"/>
+      <c r="BE47" s="106"/>
+      <c r="BF47" s="106"/>
+      <c r="BG47" s="106"/>
+      <c r="BH47" s="106"/>
+      <c r="BI47" s="106"/>
+      <c r="BJ47" s="106"/>
+      <c r="BK47" s="106"/>
+      <c r="BL47" s="106"/>
+      <c r="BM47" s="106"/>
+      <c r="BN47" s="106"/>
+    </row>
+    <row r="48" spans="1:66" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="161" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToCreateAGanttChart","► Watch How to Create a Gantt Chart in Excel")</f>
         <v>► Watch How to Create a Gantt Chart in Excel</v>
       </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="30"/>
-      <c r="N45" s="30"/>
-      <c r="O45" s="30"/>
-      <c r="P45" s="30"/>
-      <c r="Q45" s="30"/>
-      <c r="R45" s="30"/>
-      <c r="S45" s="30"/>
-      <c r="T45" s="30"/>
-      <c r="U45" s="30"/>
-      <c r="V45" s="30"/>
-      <c r="W45" s="30"/>
-      <c r="X45" s="30"/>
-      <c r="Y45" s="30"/>
-      <c r="Z45" s="30"/>
-      <c r="AA45" s="30"/>
-      <c r="AB45" s="30"/>
-      <c r="AC45" s="30"/>
-      <c r="AD45" s="30"/>
-      <c r="AE45" s="30"/>
-      <c r="AF45" s="30"/>
-      <c r="AG45" s="30"/>
-      <c r="AH45" s="30"/>
-      <c r="AI45" s="30"/>
-      <c r="AJ45" s="30"/>
-      <c r="AK45" s="30"/>
-      <c r="AL45" s="30"/>
-      <c r="AM45" s="30"/>
-      <c r="AN45" s="30"/>
-      <c r="AO45" s="30"/>
-      <c r="AP45" s="30"/>
-      <c r="AQ45" s="30"/>
-      <c r="AR45" s="30"/>
-      <c r="AS45" s="30"/>
-      <c r="AT45" s="30"/>
-      <c r="AU45" s="30"/>
-      <c r="AV45" s="30"/>
-      <c r="AW45" s="30"/>
-      <c r="AX45" s="30"/>
-      <c r="AY45" s="30"/>
-      <c r="AZ45" s="30"/>
-      <c r="BA45" s="30"/>
-      <c r="BB45" s="30"/>
-      <c r="BC45" s="30"/>
-      <c r="BD45" s="30"/>
-      <c r="BE45" s="30"/>
-      <c r="BF45" s="30"/>
-      <c r="BG45" s="30"/>
-      <c r="BH45" s="30"/>
-      <c r="BI45" s="30"/>
-      <c r="BJ45" s="30"/>
-      <c r="BK45" s="30"/>
-      <c r="BL45" s="30"/>
-      <c r="BM45" s="30"/>
-      <c r="BN45" s="30"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
+      <c r="L48" s="30"/>
+      <c r="M48" s="30"/>
+      <c r="N48" s="30"/>
+      <c r="O48" s="30"/>
+      <c r="P48" s="30"/>
+      <c r="Q48" s="30"/>
+      <c r="R48" s="30"/>
+      <c r="S48" s="30"/>
+      <c r="T48" s="30"/>
+      <c r="U48" s="30"/>
+      <c r="V48" s="30"/>
+      <c r="W48" s="30"/>
+      <c r="X48" s="30"/>
+      <c r="Y48" s="30"/>
+      <c r="Z48" s="30"/>
+      <c r="AA48" s="30"/>
+      <c r="AB48" s="30"/>
+      <c r="AC48" s="30"/>
+      <c r="AD48" s="30"/>
+      <c r="AE48" s="30"/>
+      <c r="AF48" s="30"/>
+      <c r="AG48" s="30"/>
+      <c r="AH48" s="30"/>
+      <c r="AI48" s="30"/>
+      <c r="AJ48" s="30"/>
+      <c r="AK48" s="30"/>
+      <c r="AL48" s="30"/>
+      <c r="AM48" s="30"/>
+      <c r="AN48" s="30"/>
+      <c r="AO48" s="30"/>
+      <c r="AP48" s="30"/>
+      <c r="AQ48" s="30"/>
+      <c r="AR48" s="30"/>
+      <c r="AS48" s="30"/>
+      <c r="AT48" s="30"/>
+      <c r="AU48" s="30"/>
+      <c r="AV48" s="30"/>
+      <c r="AW48" s="30"/>
+      <c r="AX48" s="30"/>
+      <c r="AY48" s="30"/>
+      <c r="AZ48" s="30"/>
+      <c r="BA48" s="30"/>
+      <c r="BB48" s="30"/>
+      <c r="BC48" s="30"/>
+      <c r="BD48" s="30"/>
+      <c r="BE48" s="30"/>
+      <c r="BF48" s="30"/>
+      <c r="BG48" s="30"/>
+      <c r="BH48" s="30"/>
+      <c r="BI48" s="30"/>
+      <c r="BJ48" s="30"/>
+      <c r="BK48" s="30"/>
+      <c r="BL48" s="30"/>
+      <c r="BM48" s="30"/>
+      <c r="BN48" s="30"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7692,10 +8141,19 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H44">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="H8:H26 H34:H47">
+    <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7709,20 +8167,209 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="3" priority="45">
+    <cfRule type="expression" dxfId="24" priority="73">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN44">
-    <cfRule type="expression" dxfId="2" priority="48">
+  <conditionalFormatting sqref="K8:BN26 K34:BN47">
+    <cfRule type="expression" dxfId="23" priority="76">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="49">
+    <cfRule type="expression" dxfId="22" priority="77">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN44">
-    <cfRule type="expression" dxfId="0" priority="8">
+  <conditionalFormatting sqref="K6:BN26 K34:BN47">
+    <cfRule type="expression" dxfId="21" priority="36">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
+    <cfRule type="dataBar" priority="25">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{34362A0D-F701-4474-ADAF-21BE291869DE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27:BN27">
+    <cfRule type="expression" dxfId="20" priority="27">
+      <formula>AND($E27&lt;=K$6,ROUNDDOWN(($F27-$E27+1)*$H27,0)+$E27-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="28">
+      <formula>AND(NOT(ISBLANK($E27)),$E27&lt;=K$6,$F27&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27:BN27">
+    <cfRule type="expression" dxfId="18" priority="26">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28">
+    <cfRule type="dataBar" priority="21">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{66005769-C478-4CDF-B831-1FCD8509CBDB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28:BN28">
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>AND($E28&lt;=K$6,ROUNDDOWN(($F28-$E28+1)*$H28,0)+$E28-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>AND(NOT(ISBLANK($E28)),$E28&lt;=K$6,$F28&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28:BN28">
+    <cfRule type="expression" dxfId="15" priority="22">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29">
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{79DE39A2-8D7C-4D03-88BB-8ED156CAC480}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29:BN29">
+    <cfRule type="expression" dxfId="14" priority="19">
+      <formula>AND($E29&lt;=K$6,ROUNDDOWN(($F29-$E29+1)*$H29,0)+$E29-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="20">
+      <formula>AND(NOT(ISBLANK($E29)),$E29&lt;=K$6,$F29&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29:BN29">
+    <cfRule type="expression" dxfId="12" priority="18">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C4A08678-FBD4-4E40-B2EF-B2AA59E1FBC4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30:BN30">
+    <cfRule type="expression" dxfId="11" priority="15">
+      <formula>AND($E30&lt;=K$6,ROUNDDOWN(($F30-$E30+1)*$H30,0)+$E30-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="16">
+      <formula>AND(NOT(ISBLANK($E30)),$E30&lt;=K$6,$F30&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30:BN30">
+    <cfRule type="expression" dxfId="9" priority="14">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2D32C774-CFC0-45DF-8F53-58A7A152FF0F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31:BN31">
+    <cfRule type="expression" dxfId="8" priority="11">
+      <formula>AND($E31&lt;=K$6,ROUNDDOWN(($F31-$E31+1)*$H31,0)+$E31-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="12">
+      <formula>AND(NOT(ISBLANK($E31)),$E31&lt;=K$6,$F31&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31:BN31">
+    <cfRule type="expression" dxfId="6" priority="10">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{89B1A9F7-C28C-4AD8-894A-4785485FC4AD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32:BN32">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>AND($E32&lt;=K$6,ROUNDDOWN(($F32-$E32+1)*$H32,0)+$E32-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>AND(NOT(ISBLANK($E32)),$E32&lt;=K$6,$F32&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32:BN32">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{26D74C39-8E84-4882-ADF2-F3F3AEB813A7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33:BN33">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND($E33&lt;=K$6,ROUNDDOWN(($F33-$E33+1)*$H33,0)+$E33-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>AND(NOT(ISBLANK($E33)),$E33&lt;=K$6,$F33&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33:BN33">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7736,8 +8383,8 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A37:B38 B32 B33:B35 B27:B29 A40:B40 B39 E18 E25 E31 E38:H40 G18:H18 G25:H25 G31:H35 G41 G42:G43 G44 H26:H29 F37:H37" unlockedFormula="1"/>
-    <ignoredError sqref="A31 A25 A18" formula="1"/>
+    <ignoredError sqref="H9 A40:B41 B35 B36:B38 A43:B43 B42 E18 E25 E34 E41:H43 G18:H18 G25:H25 G34:H38 G44 G45:G46 G47 F40:H40" unlockedFormula="1"/>
+    <ignoredError sqref="A34 A25 A18" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -7751,13 +8398,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>95250</xdr:colOff>
+                    <xdr:colOff>99060</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>27</xdr:col>
-                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:colOff>106680</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </to>
@@ -7785,7 +8432,112 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H44</xm:sqref>
+          <xm:sqref>H8:H26 H34:H47</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{34362A0D-F701-4474-ADAF-21BE291869DE}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{66005769-C478-4CDF-B831-1FCD8509CBDB}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{79DE39A2-8D7C-4D03-88BB-8ED156CAC480}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C4A08678-FBD4-4E40-B2EF-B2AA59E1FBC4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2D32C774-CFC0-45DF-8F53-58A7A152FF0F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{89B1A9F7-C28C-4AD8-894A-4785485FC4AD}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{26D74C39-8E84-4882-ADF2-F3F3AEB813A7}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -7804,175 +8556,175 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" style="16" customWidth="1"/>
-    <col min="4" max="7" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="5.5546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="55.109375" style="16" customWidth="1"/>
+    <col min="4" max="7" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="20"/>
     </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C7" s="24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C13" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B34" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="20" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="20" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B39" s="26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B42" s="26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="20" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B46" s="24" t="s">
         <v>25</v>
       </c>
@@ -7998,74 +8750,74 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="90.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="7"/>
+    <col min="1" max="1" width="5.5546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="90.44140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>125</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="41"/>
     </row>
-    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="136" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="131" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="38"/>
     </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="8" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B5" s="137" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B7" s="137" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B9" s="136" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B11" s="135" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="175" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="175"/>
     </row>
-    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:3" s="132" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" s="132" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="140"/>
       <c r="B15" s="138" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="132" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="132" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A16" s="140"/>
       <c r="B16" s="139" t="s">
         <v>82</v>
@@ -8074,25 +8826,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="141"/>
       <c r="B17" s="139" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="20" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="141"/>
       <c r="B18" s="139" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="41" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="41" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="144"/>
       <c r="B19" s="139" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="132" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="132" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="140"/>
       <c r="B20" s="138" t="s">
         <v>83</v>
@@ -8101,153 +8853,153 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="141"/>
       <c r="B21" s="139" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="142"/>
       <c r="B22" s="143" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="142"/>
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="175" t="s">
         <v>88</v>
       </c>
       <c r="B24" s="175"/>
     </row>
-    <row r="25" spans="1:3" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="8" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A25" s="142"/>
       <c r="B25" s="139" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="142"/>
       <c r="B26" s="139"/>
     </row>
-    <row r="27" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="142"/>
       <c r="B27" s="160" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="142"/>
       <c r="B28" s="139" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="142"/>
       <c r="B29" s="139" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="142"/>
       <c r="B30" s="139"/>
     </row>
-    <row r="31" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="142"/>
       <c r="B31" s="160" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="142"/>
       <c r="B32" s="139" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="142"/>
       <c r="B33" s="139" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="142"/>
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A35" s="142"/>
       <c r="B35" s="139" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="142"/>
       <c r="B36" s="145" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="142"/>
       <c r="B37" s="10"/>
     </row>
-    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="175" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="175"/>
     </row>
-    <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B39" s="139" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:2" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B41" s="139" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:2" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:2" s="20" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B43" s="139" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B45" s="139" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" s="21"/>
     </row>
-    <row r="47" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B47" s="139" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" s="11"/>
     </row>
-    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" s="175" t="s">
         <v>8</v>
       </c>
       <c r="B49" s="175"/>
     </row>
-    <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B50" s="139" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" s="11"/>
     </row>
-    <row r="52" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A52" s="146" t="s">
         <v>13</v>
       </c>
@@ -8255,7 +9007,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A53" s="146" t="s">
         <v>15</v>
       </c>
@@ -8263,7 +9015,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A54" s="146" t="s">
         <v>17</v>
       </c>
@@ -8271,19 +9023,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A55" s="135"/>
       <c r="B55" s="139" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A56" s="135"/>
       <c r="B56" s="139" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A57" s="146" t="s">
         <v>19</v>
       </c>
@@ -8291,19 +9043,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A58" s="135"/>
       <c r="B58" s="139" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A59" s="135"/>
       <c r="B59" s="139" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A60" s="146" t="s">
         <v>21</v>
       </c>
@@ -8311,13 +9063,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A61" s="135"/>
       <c r="B61" s="139" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A62" s="146" t="s">
         <v>111</v>
       </c>
@@ -8325,36 +9077,36 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A63" s="147"/>
       <c r="B63" s="139" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="12"/>
     </row>
-    <row r="65" spans="1:2" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" s="20" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A65" s="175" t="s">
         <v>11</v>
       </c>
       <c r="B65" s="175"/>
     </row>
-    <row r="66" spans="1:2" s="20" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" s="20" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B66" s="139" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="13"/>
     </row>
-    <row r="68" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A68" s="175" t="s">
         <v>6</v>
       </c>
       <c r="B68" s="175"/>
     </row>
-    <row r="69" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A69" s="154" t="s">
         <v>7</v>
       </c>
@@ -8362,17 +9114,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A70" s="148"/>
       <c r="B70" s="153" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A71" s="148"/>
       <c r="B71" s="149"/>
     </row>
-    <row r="72" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A72" s="154" t="s">
         <v>7</v>
       </c>
@@ -8380,17 +9132,17 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A73" s="148"/>
       <c r="B73" s="153" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A74" s="148"/>
       <c r="B74" s="149"/>
     </row>
-    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A75" s="154" t="s">
         <v>7</v>
       </c>
@@ -8398,17 +9150,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" s="8" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A76" s="148"/>
       <c r="B76" s="137" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A77" s="147"/>
       <c r="B77" s="147"/>
     </row>
-    <row r="78" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A78" s="154" t="s">
         <v>7</v>
       </c>
@@ -8416,17 +9168,17 @@
         <v>126</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A79" s="148"/>
       <c r="B79" s="137" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" s="20" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A80" s="147"/>
       <c r="B80" s="147"/>
     </row>
-    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A81" s="154" t="s">
         <v>7</v>
       </c>
@@ -8434,29 +9186,29 @@
         <v>127</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A82" s="148"/>
       <c r="B82" s="152" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A83" s="148"/>
       <c r="B83" s="152" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A84" s="148"/>
       <c r="B84" s="152" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A85" s="147"/>
       <c r="B85" s="151"/>
     </row>
-    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A86" s="154" t="s">
         <v>7</v>
       </c>
@@ -8464,29 +9216,29 @@
         <v>128</v>
       </c>
     </row>
-    <row r="87" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" s="8" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A87" s="148"/>
       <c r="B87" s="137" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A88" s="148"/>
       <c r="B88" s="150" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="1:2" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" s="8" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A89" s="148"/>
       <c r="B89" s="156" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A90" s="147"/>
       <c r="B90" s="147"/>
     </row>
-    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A91" s="154" t="s">
         <v>7</v>
       </c>
@@ -8494,13 +9246,13 @@
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A92" s="135"/>
       <c r="B92" s="152" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="28" t="s">
         <v>56</v>
       </c>
@@ -8536,14 +9288,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="20" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="5.5546875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="82.109375" style="20" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>54</v>
       </c>
@@ -8551,163 +9303,163 @@
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="41"/>
       <c r="B2" s="45"/>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="42"/>
       <c r="B3" s="35" t="s">
         <v>55</v>
       </c>
       <c r="C3" s="43"/>
     </row>
-    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="37" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="15"/>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="17"/>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="18" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="17"/>
       <c r="C7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="17" t="s">
         <v>57</v>
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="17"/>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="46.2" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="17" t="s">
         <v>58</v>
       </c>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="17"/>
       <c r="C11" s="15"/>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="17" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="15"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="17" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:4" ht="30.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="30.6" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="17" t="s">
         <v>61</v>
       </c>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="36" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="19"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>

</xml_diff>